<commit_message>
Added switching mirror on the LAPP Main Branch to setupChannel
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukhina\Documents\MATLAB\ScopeScript-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE2A49-4B31-4C15-9B88-0DF3C8F3017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A01384-1E58-4F48-AA55-2DADBFB70571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{64517161-2A91-2B47-8856-8DF463AC8E32}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Arduino code check list" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$215</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="251">
   <si>
     <r>
       <t>Left file list</t>
@@ -2222,12 +2222,24 @@
   <si>
     <t>constantPiezoLightsOn.m</t>
   </si>
+  <si>
+    <t>"Fast USB to Serial" --&gt; enabled for COM7 (Toptica) and COM4 (Arduino)</t>
+  </si>
+  <si>
+    <t>!!!!CHECK FOR STABILITY - supposed to speed up communication by 10x</t>
+  </si>
+  <si>
+    <t>mapChannelToMirrorPosition</t>
+  </si>
+  <si>
+    <t>getMirrorPosition()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2419,6 +2431,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2479,7 +2504,7 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2512,6 +2537,13 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2521,9 +2553,6 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2892,11 +2921,11 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:H213"/>
+  <dimension ref="A1:H215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A150" sqref="A150:XFD150"/>
+      <pane ySplit="8" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125:XFD125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2937,14 +2966,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
@@ -2984,10 +3013,10 @@
       <c r="A10" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="22">
         <v>835</v>
       </c>
@@ -3005,10 +3034,10 @@
       <c r="A11" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="22">
         <v>2953</v>
       </c>
@@ -3026,10 +3055,10 @@
       <c r="A12" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="22">
         <v>406</v>
       </c>
@@ -3047,10 +3076,10 @@
       <c r="A13" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="22">
         <v>5488</v>
       </c>
@@ -3068,10 +3097,10 @@
       <c r="A14" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="34"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="22">
         <v>634</v>
       </c>
@@ -3089,10 +3118,10 @@
       <c r="A15" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="22">
         <v>510</v>
       </c>
@@ -3110,10 +3139,10 @@
       <c r="A16" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="22">
         <v>771</v>
       </c>
@@ -3131,10 +3160,10 @@
       <c r="A17" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="22">
         <v>1203</v>
       </c>
@@ -3152,10 +3181,10 @@
       <c r="A18" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="22">
         <v>594</v>
       </c>
@@ -3173,10 +3202,10 @@
       <c r="A19" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="22">
         <v>962</v>
       </c>
@@ -3194,10 +3223,10 @@
       <c r="A20" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="22">
         <v>1255</v>
       </c>
@@ -3215,10 +3244,10 @@
       <c r="A21" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="22">
         <v>2288</v>
       </c>
@@ -3236,10 +3265,10 @@
       <c r="A22" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="22">
         <v>1552</v>
       </c>
@@ -3257,10 +3286,10 @@
       <c r="A23" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="34"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="22">
         <v>764</v>
       </c>
@@ -3278,10 +3307,10 @@
       <c r="A24" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="34"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="22">
         <v>342</v>
       </c>
@@ -4202,10 +4231,10 @@
       <c r="A67" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="31" t="s">
+      <c r="B67" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="31"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="17">
         <v>314</v>
       </c>
@@ -4220,10 +4249,10 @@
       <c r="A68" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="31"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="17">
         <v>308</v>
       </c>
@@ -4343,10 +4372,10 @@
       <c r="A75" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="31" t="s">
+      <c r="B75" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="31"/>
+      <c r="C75" s="34"/>
       <c r="D75" s="17">
         <v>286</v>
       </c>
@@ -4384,10 +4413,10 @@
       <c r="A77" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B77" s="33" t="s">
+      <c r="B77" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="33"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="7">
         <v>833</v>
       </c>
@@ -4465,10 +4494,10 @@
       <c r="A81" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B81" s="33" t="s">
+      <c r="B81" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="33"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="7">
         <v>2626</v>
       </c>
@@ -4690,10 +4719,10 @@
       <c r="A94" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="32" t="s">
+      <c r="B94" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="32"/>
+      <c r="C94" s="35"/>
       <c r="D94" s="17">
         <v>709</v>
       </c>
@@ -5008,10 +5037,10 @@
       <c r="A112" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B112" s="30" t="s">
+      <c r="B112" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C112" s="30"/>
+      <c r="C112" s="33"/>
       <c r="D112" s="20">
         <v>1225</v>
       </c>
@@ -5026,10 +5055,10 @@
       <c r="A113" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B113" s="30" t="s">
+      <c r="B113" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C113" s="30"/>
+      <c r="C113" s="33"/>
       <c r="D113" s="20">
         <v>1053</v>
       </c>
@@ -5044,10 +5073,10 @@
       <c r="A114" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B114" s="31" t="s">
+      <c r="B114" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C114" s="31"/>
+      <c r="C114" s="34"/>
       <c r="D114" s="17">
         <v>6709</v>
       </c>
@@ -5224,77 +5253,55 @@
     </row>
     <row r="125" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="29" t="s">
-        <v>188</v>
+        <v>250</v>
       </c>
       <c r="C125" s="14"/>
       <c r="F125" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A126" s="28" t="s">
+    <row r="126" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C126" s="14"/>
+      <c r="F126" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="C127" s="14"/>
+      <c r="F127" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+      <c r="A128" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B126" s="3"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="5"/>
-      <c r="F126" s="11"/>
-    </row>
-    <row r="127" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A127" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B127" s="13">
-        <v>257</v>
-      </c>
-      <c r="C127" s="14">
-        <v>45533.322002314817</v>
-      </c>
-      <c r="D127" s="13">
-        <v>257</v>
-      </c>
-      <c r="E127" s="14">
-        <v>42978.469814814816</v>
-      </c>
-      <c r="F127" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A128" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B128" s="13">
-        <v>536</v>
-      </c>
-      <c r="C128" s="14">
-        <v>45533.322002314817</v>
-      </c>
-      <c r="D128" s="13">
-        <v>536</v>
-      </c>
-      <c r="E128" s="14">
-        <v>42978.465370370373</v>
-      </c>
-      <c r="F128" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="5"/>
+      <c r="F128" s="11"/>
     </row>
     <row r="129" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B129" s="13">
-        <v>472</v>
+        <v>257</v>
       </c>
       <c r="C129" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D129" s="13">
-        <v>472</v>
+        <v>257</v>
       </c>
       <c r="E129" s="14">
-        <v>43041.741759259261</v>
+        <v>42978.469814814816</v>
       </c>
       <c r="F129" s="13" t="s">
         <v>11</v>
@@ -5302,19 +5309,19 @@
     </row>
     <row r="130" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B130" s="13">
-        <v>257</v>
+        <v>536</v>
       </c>
       <c r="C130" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D130" s="13">
-        <v>257</v>
+        <v>536</v>
       </c>
       <c r="E130" s="14">
-        <v>42978.510162037041</v>
+        <v>42978.465370370373</v>
       </c>
       <c r="F130" s="13" t="s">
         <v>11</v>
@@ -5322,19 +5329,19 @@
     </row>
     <row r="131" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B131" s="13">
-        <v>741</v>
+        <v>472</v>
       </c>
       <c r="C131" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D131" s="13">
-        <v>741</v>
+        <v>472</v>
       </c>
       <c r="E131" s="14">
-        <v>42978.451574074075</v>
+        <v>43041.741759259261</v>
       </c>
       <c r="F131" s="13" t="s">
         <v>11</v>
@@ -5342,19 +5349,19 @@
     </row>
     <row r="132" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B132" s="13">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="C132" s="14">
-        <v>45533.322013888886</v>
+        <v>45533.322002314817</v>
       </c>
       <c r="D132" s="13">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="E132" s="14">
-        <v>44865.577453703707</v>
+        <v>42978.510162037041</v>
       </c>
       <c r="F132" s="13" t="s">
         <v>11</v>
@@ -5362,19 +5369,19 @@
     </row>
     <row r="133" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B133" s="13">
-        <v>77</v>
+        <v>741</v>
       </c>
       <c r="C133" s="14">
-        <v>45533.322013888886</v>
+        <v>45533.322002314817</v>
       </c>
       <c r="D133" s="13">
-        <v>77</v>
+        <v>741</v>
       </c>
       <c r="E133" s="14">
-        <v>42977.54828703704</v>
+        <v>42978.451574074075</v>
       </c>
       <c r="F133" s="13" t="s">
         <v>11</v>
@@ -5382,19 +5389,19 @@
     </row>
     <row r="134" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B134" s="13">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C134" s="14">
         <v>45533.322013888886</v>
       </c>
       <c r="D134" s="13">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E134" s="14">
-        <v>42992.41233796296</v>
+        <v>44865.577453703707</v>
       </c>
       <c r="F134" s="13" t="s">
         <v>11</v>
@@ -5402,85 +5409,79 @@
     </row>
     <row r="135" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B135" s="13">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="C135" s="14">
         <v>45533.322013888886</v>
       </c>
       <c r="D135" s="13">
+        <v>77</v>
+      </c>
+      <c r="E135" s="14">
+        <v>42977.54828703704</v>
+      </c>
+      <c r="F135" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A136" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B136" s="13">
+        <v>125</v>
+      </c>
+      <c r="C136" s="14">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D136" s="13">
+        <v>125</v>
+      </c>
+      <c r="E136" s="14">
+        <v>42992.41233796296</v>
+      </c>
+      <c r="F136" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" s="13">
         <v>310</v>
       </c>
-      <c r="E135" s="14">
+      <c r="C137" s="14">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D137" s="13">
+        <v>310</v>
+      </c>
+      <c r="E137" s="14">
         <v>44865.57775462963</v>
       </c>
-      <c r="F135" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A136" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B136" s="15">
-        <v>386</v>
-      </c>
-      <c r="C136" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D136" s="15">
-        <v>386</v>
-      </c>
-      <c r="E136" s="16">
-        <v>44865.615277777775</v>
-      </c>
-      <c r="F136" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H136" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B137" s="15">
-        <v>264</v>
-      </c>
-      <c r="C137" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D137" s="15">
-        <v>264</v>
-      </c>
-      <c r="E137" s="16">
-        <v>42989.788611111115</v>
-      </c>
-      <c r="F137" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H137" s="15" t="s">
-        <v>225</v>
+      <c r="F137" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B138" s="15">
-        <v>232</v>
+        <v>386</v>
       </c>
       <c r="C138" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D138" s="15">
-        <v>232</v>
+        <v>386</v>
       </c>
       <c r="E138" s="16">
-        <v>44865.616296296299</v>
+        <v>44865.615277777775</v>
       </c>
       <c r="F138" s="15" t="s">
         <v>11</v>
@@ -5491,19 +5492,19 @@
     </row>
     <row r="139" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B139" s="15">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="C139" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D139" s="15">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="E139" s="16">
-        <v>42989.793263888889</v>
+        <v>42989.788611111115</v>
       </c>
       <c r="F139" s="15" t="s">
         <v>11</v>
@@ -5514,19 +5515,19 @@
     </row>
     <row r="140" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B140" s="15">
-        <v>1048</v>
+        <v>232</v>
       </c>
       <c r="C140" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D140" s="15">
-        <v>1048</v>
+        <v>232</v>
       </c>
       <c r="E140" s="16">
-        <v>44869.567465277774</v>
+        <v>44865.616296296299</v>
       </c>
       <c r="F140" s="15" t="s">
         <v>11</v>
@@ -5537,19 +5538,19 @@
     </row>
     <row r="141" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B141" s="15">
-        <v>130</v>
+        <v>284</v>
       </c>
       <c r="C141" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D141" s="15">
-        <v>130</v>
+        <v>284</v>
       </c>
       <c r="E141" s="16">
-        <v>44865.584699074076</v>
+        <v>42989.793263888889</v>
       </c>
       <c r="F141" s="15" t="s">
         <v>11</v>
@@ -5560,19 +5561,19 @@
     </row>
     <row r="142" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A142" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B142" s="15">
-        <v>468</v>
+        <v>1048</v>
       </c>
       <c r="C142" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D142" s="15">
-        <v>468</v>
+        <v>1048</v>
       </c>
       <c r="E142" s="16">
-        <v>44865.591597222221</v>
+        <v>44869.567465277774</v>
       </c>
       <c r="F142" s="15" t="s">
         <v>11</v>
@@ -5581,286 +5582,292 @@
         <v>225</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A143" s="27" t="s">
+    <row r="143" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B143" s="15">
+        <v>130</v>
+      </c>
+      <c r="C143" s="16">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D143" s="15">
+        <v>130</v>
+      </c>
+      <c r="E143" s="16">
+        <v>44865.584699074076</v>
+      </c>
+      <c r="F143" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H143" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B144" s="15">
+        <v>468</v>
+      </c>
+      <c r="C144" s="16">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D144" s="15">
+        <v>468</v>
+      </c>
+      <c r="E144" s="16">
+        <v>44865.591597222221</v>
+      </c>
+      <c r="F144" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H144" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A145" s="27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="22" t="s">
+    <row r="146" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="B144" s="22">
+      <c r="B146" s="22">
         <v>2387</v>
       </c>
-      <c r="C144" s="23">
+      <c r="C146" s="23">
         <v>45533.322013888886</v>
       </c>
-      <c r="D144" s="22">
+      <c r="D146" s="22">
         <v>2387</v>
       </c>
-      <c r="E144" s="23">
+      <c r="E146" s="23">
         <v>44862.525694444441</v>
       </c>
-      <c r="F144" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A145" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B145" s="13">
-        <v>156</v>
-      </c>
-      <c r="C145" s="14">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D145" s="13">
-        <v>156</v>
-      </c>
-      <c r="E145" s="14">
-        <v>42949.567870370367</v>
-      </c>
-      <c r="F145" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A146" s="27" t="s">
-        <v>135</v>
+      <c r="F146" s="22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A147" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B147" s="13">
+        <v>156</v>
+      </c>
+      <c r="C147" s="14">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D147" s="13">
+        <v>156</v>
+      </c>
+      <c r="E147" s="14">
+        <v>42949.567870370367</v>
+      </c>
+      <c r="F147" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A148" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="F147" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H147" s="13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="F148" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H148" s="13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A149" s="29" t="s">
-        <v>239</v>
       </c>
       <c r="F149" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B150" s="20">
-        <v>260</v>
-      </c>
-      <c r="C150" s="20">
-        <v>45533.32203703704</v>
-      </c>
-      <c r="D150" s="20">
-        <v>260</v>
-      </c>
-      <c r="E150" s="20">
-        <v>44865.684282407405</v>
-      </c>
-      <c r="F150" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H150" s="20" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F150" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H150" s="13" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="C151" s="14"/>
-      <c r="E151" s="14"/>
+      <c r="A151" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="F151" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H151" s="13" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="152" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A152" s="20" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B152" s="20">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C152" s="20">
         <v>45533.32203703704</v>
       </c>
       <c r="D152" s="20">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E152" s="20">
-        <v>44868.638414351852</v>
+        <v>44865.684282407405</v>
       </c>
       <c r="F152" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H152" s="20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A153" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A154" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B154" s="20">
+        <v>265</v>
+      </c>
+      <c r="C154" s="20">
+        <v>45533.32203703704</v>
+      </c>
+      <c r="D154" s="20">
+        <v>265</v>
+      </c>
+      <c r="E154" s="20">
+        <v>44868.638414351852</v>
+      </c>
+      <c r="F154" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H154" s="20" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="153" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="20" t="s">
+    <row r="155" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="B153" s="20">
+      <c r="B155" s="20">
         <v>275</v>
       </c>
-      <c r="C153" s="20">
+      <c r="C155" s="20">
         <v>45533.32203703704</v>
       </c>
-      <c r="D153" s="20">
+      <c r="D155" s="20">
         <v>275</v>
       </c>
-      <c r="E153" s="20">
+      <c r="E155" s="20">
         <v>44868.639050925929</v>
       </c>
-      <c r="F153" s="20" t="s">
+      <c r="F155" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H153" s="20" t="s">
+      <c r="H155" s="20" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="154" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A154" s="13" t="s">
+    <row r="156" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B154" s="13">
+      <c r="B156" s="13">
         <v>1257</v>
       </c>
-      <c r="C154" s="14">
+      <c r="C156" s="14">
         <v>45636.738125000003</v>
       </c>
-      <c r="D154" s="13">
+      <c r="D156" s="13">
         <v>749</v>
       </c>
-      <c r="E154" s="14">
+      <c r="E156" s="14">
         <v>44865.678263888891</v>
       </c>
-      <c r="F154" s="13" t="s">
+      <c r="F156" s="13" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A155" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B155" s="13">
-        <v>906</v>
-      </c>
-      <c r="C155" s="14">
-        <v>45636.727048611108</v>
-      </c>
-      <c r="D155" s="13">
-        <v>767</v>
-      </c>
-      <c r="E155" s="14">
-        <v>44865.681134259263</v>
-      </c>
-      <c r="F155" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A156" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B156" s="15">
-        <v>1057</v>
-      </c>
-      <c r="C156" s="16">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D156" s="15">
-        <v>1057</v>
-      </c>
-      <c r="E156" s="16">
-        <v>44865.684537037036</v>
-      </c>
-      <c r="F156" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H156" s="15" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B157" s="13">
-        <v>358</v>
+        <v>906</v>
       </c>
       <c r="C157" s="14">
+        <v>45636.727048611108</v>
+      </c>
+      <c r="D157" s="13">
+        <v>767</v>
+      </c>
+      <c r="E157" s="14">
+        <v>44865.681134259263</v>
+      </c>
+      <c r="F157" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B158" s="15">
+        <v>1057</v>
+      </c>
+      <c r="C158" s="16">
         <v>45533.322048611109</v>
       </c>
-      <c r="D157" s="13">
-        <v>358</v>
-      </c>
-      <c r="E157" s="14">
-        <v>44865.660231481481</v>
-      </c>
-      <c r="F157" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A158" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="B158" s="13">
-        <v>365</v>
-      </c>
-      <c r="C158" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D158" s="13">
-        <v>365</v>
-      </c>
-      <c r="E158" s="14">
-        <v>44865.659814814811</v>
-      </c>
-      <c r="F158" s="13" t="s">
-        <v>11</v>
+      <c r="D158" s="15">
+        <v>1057</v>
+      </c>
+      <c r="E158" s="16">
+        <v>44865.684537037036</v>
+      </c>
+      <c r="F158" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H158" s="15" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B159" s="13">
-        <v>563</v>
+        <v>358</v>
       </c>
       <c r="C159" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D159" s="13">
-        <v>563</v>
+        <v>358</v>
       </c>
       <c r="E159" s="14">
-        <v>44865.672083333331</v>
+        <v>44865.660231481481</v>
       </c>
       <c r="F159" s="13" t="s">
         <v>11</v>
@@ -5868,202 +5875,202 @@
     </row>
     <row r="160" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" s="13" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B160" s="13">
-        <v>253</v>
+        <v>365</v>
       </c>
       <c r="C160" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D160" s="13">
-        <v>253</v>
+        <v>365</v>
       </c>
       <c r="E160" s="14">
-        <v>44865.664467592593</v>
+        <v>44865.659814814811</v>
       </c>
       <c r="F160" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A161" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="B161" s="22">
-        <v>1062</v>
-      </c>
-      <c r="C161" s="23">
+    <row r="161" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A161" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B161" s="13">
+        <v>563</v>
+      </c>
+      <c r="C161" s="14">
         <v>45533.322048611109</v>
       </c>
-      <c r="D161" s="22">
-        <v>1062</v>
-      </c>
-      <c r="E161" s="23">
-        <v>44865.663032407407</v>
-      </c>
-      <c r="F161" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H161" s="36" t="s">
-        <v>233</v>
+      <c r="D161" s="13">
+        <v>563</v>
+      </c>
+      <c r="E161" s="14">
+        <v>44865.672083333331</v>
+      </c>
+      <c r="F161" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B162" s="13">
-        <v>499</v>
+        <v>253</v>
       </c>
       <c r="C162" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D162" s="13">
-        <v>499</v>
+        <v>253</v>
       </c>
       <c r="E162" s="14">
-        <v>44846.595578703702</v>
+        <v>44865.664467592593</v>
       </c>
       <c r="F162" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B163" s="13">
-        <v>285</v>
-      </c>
-      <c r="C163" s="14">
+    <row r="163" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B163" s="22">
+        <v>1062</v>
+      </c>
+      <c r="C163" s="23">
         <v>45533.322048611109</v>
       </c>
-      <c r="D163" s="13">
-        <v>285</v>
-      </c>
-      <c r="E163" s="14">
-        <v>44846.595578703702</v>
-      </c>
-      <c r="F163" s="13" t="s">
-        <v>11</v>
+      <c r="D163" s="22">
+        <v>1062</v>
+      </c>
+      <c r="E163" s="23">
+        <v>44865.663032407407</v>
+      </c>
+      <c r="F163" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H163" s="30" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" s="13" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B164" s="13">
-        <v>989</v>
+        <v>499</v>
       </c>
       <c r="C164" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D164" s="13">
-        <v>989</v>
+        <v>499</v>
       </c>
       <c r="E164" s="14">
-        <v>44865.669976851852</v>
+        <v>44846.595578703702</v>
       </c>
       <c r="F164" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A165" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B165" s="3"/>
-      <c r="C165" s="6"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="6"/>
-      <c r="F165" s="11"/>
+    <row r="165" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A165" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B165" s="13">
+        <v>285</v>
+      </c>
+      <c r="C165" s="14">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D165" s="13">
+        <v>285</v>
+      </c>
+      <c r="E165" s="14">
+        <v>44846.595578703702</v>
+      </c>
+      <c r="F165" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="166" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A166" s="13" t="s">
-        <v>137</v>
+        <v>220</v>
       </c>
       <c r="B166" s="13">
-        <v>329</v>
+        <v>989</v>
       </c>
       <c r="C166" s="14">
-        <v>45637.51290509259</v>
+        <v>45533.322048611109</v>
       </c>
       <c r="D166" s="13">
-        <v>418</v>
+        <v>989</v>
       </c>
       <c r="E166" s="14">
-        <v>44869.465717592589</v>
+        <v>44865.669976851852</v>
       </c>
       <c r="F166" s="13" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A167" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B167" s="3"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="3"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="11"/>
+    </row>
+    <row r="168" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A168" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B168" s="13">
+        <v>329</v>
+      </c>
+      <c r="C168" s="14">
+        <v>45637.51290509259</v>
+      </c>
+      <c r="D168" s="13">
+        <v>418</v>
+      </c>
+      <c r="E168" s="14">
+        <v>44869.465717592589</v>
+      </c>
+      <c r="F168" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A169" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A168" s="28" t="s">
+    <row r="170" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A170" s="28" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A169" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B169" s="3">
-        <v>181</v>
-      </c>
-      <c r="C169" s="6">
-        <v>45533.322071759256</v>
-      </c>
-      <c r="D169" s="3">
-        <v>181</v>
-      </c>
-      <c r="E169" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F169" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A170" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B170" s="3">
-        <v>242</v>
-      </c>
-      <c r="C170" s="6">
-        <v>45533.322071759256</v>
-      </c>
-      <c r="D170" s="3">
-        <v>242</v>
-      </c>
-      <c r="E170" s="6">
-        <v>43763.840231481481</v>
-      </c>
-      <c r="F170" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A171" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B171" s="3">
-        <v>1778</v>
+        <v>181</v>
       </c>
       <c r="C171" s="6">
         <v>45533.322071759256</v>
       </c>
       <c r="D171" s="3">
-        <v>1778</v>
+        <v>181</v>
       </c>
       <c r="E171" s="6">
-        <v>44868.696817129632</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F171" s="11" t="s">
         <v>11</v>
@@ -6071,19 +6078,19 @@
     </row>
     <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A172" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B172" s="3">
-        <v>1520</v>
+        <v>242</v>
       </c>
       <c r="C172" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322071759256</v>
       </c>
       <c r="D172" s="3">
-        <v>1520</v>
+        <v>242</v>
       </c>
       <c r="E172" s="6">
-        <v>42949.567847222221</v>
+        <v>43763.840231481481</v>
       </c>
       <c r="F172" s="11" t="s">
         <v>11</v>
@@ -6091,19 +6098,19 @@
     </row>
     <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A173" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B173" s="3">
-        <v>791</v>
+        <v>1778</v>
       </c>
       <c r="C173" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322071759256</v>
       </c>
       <c r="D173" s="3">
-        <v>791</v>
+        <v>1778</v>
       </c>
       <c r="E173" s="6">
-        <v>42949.567847222221</v>
+        <v>44868.696817129632</v>
       </c>
       <c r="F173" s="11" t="s">
         <v>11</v>
@@ -6111,19 +6118,19 @@
     </row>
     <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A174" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B174" s="3">
-        <v>761</v>
+        <v>1520</v>
       </c>
       <c r="C174" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D174" s="3">
-        <v>761</v>
+        <v>1520</v>
       </c>
       <c r="E174" s="6">
-        <v>42990.771851851852</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F174" s="11" t="s">
         <v>11</v>
@@ -6131,16 +6138,16 @@
     </row>
     <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A175" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B175" s="3">
-        <v>173</v>
+        <v>791</v>
       </c>
       <c r="C175" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D175" s="3">
-        <v>173</v>
+        <v>791</v>
       </c>
       <c r="E175" s="6">
         <v>42949.567847222221</v>
@@ -6151,102 +6158,102 @@
     </row>
     <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A176" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B176" s="3">
-        <v>1710</v>
+        <v>761</v>
       </c>
       <c r="C176" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D176" s="3">
-        <v>1710</v>
+        <v>761</v>
       </c>
       <c r="E176" s="6">
-        <v>43711.608078703706</v>
+        <v>42990.771851851852</v>
       </c>
       <c r="F176" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A177" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B177" s="22">
-        <v>3385</v>
-      </c>
-      <c r="C177" s="23">
-        <v>45637.536157407405</v>
-      </c>
-      <c r="D177" s="22">
-        <v>3379</v>
-      </c>
-      <c r="E177" s="23">
-        <v>44865.695879629631</v>
-      </c>
-      <c r="F177" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H177" s="22" t="s">
-        <v>233</v>
+    <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A177" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B177" s="3">
+        <v>173</v>
+      </c>
+      <c r="C177" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D177" s="3">
+        <v>173</v>
+      </c>
+      <c r="E177" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F177" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A178" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B178" s="3">
-        <v>261</v>
+        <v>1710</v>
       </c>
       <c r="C178" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D178" s="3">
-        <v>261</v>
+        <v>1710</v>
       </c>
       <c r="E178" s="6">
-        <v>42949.567847222221</v>
+        <v>43711.608078703706</v>
       </c>
       <c r="F178" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A179" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B179" s="3">
-        <v>876</v>
-      </c>
-      <c r="C179" s="6">
-        <v>45533.322083333333</v>
-      </c>
-      <c r="D179" s="3">
-        <v>876</v>
-      </c>
-      <c r="E179" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F179" s="11" t="s">
-        <v>11</v>
+    <row r="179" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A179" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B179" s="22">
+        <v>3385</v>
+      </c>
+      <c r="C179" s="23">
+        <v>45637.536157407405</v>
+      </c>
+      <c r="D179" s="22">
+        <v>3379</v>
+      </c>
+      <c r="E179" s="23">
+        <v>44865.695879629631</v>
+      </c>
+      <c r="F179" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H179" s="22" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A180" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B180" s="3">
-        <v>571</v>
+        <v>261</v>
       </c>
       <c r="C180" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D180" s="3">
-        <v>571</v>
+        <v>261</v>
       </c>
       <c r="E180" s="6">
-        <v>44076.622754629629</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F180" s="11" t="s">
         <v>11</v>
@@ -6254,102 +6261,102 @@
     </row>
     <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A181" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B181" s="3">
-        <v>1122</v>
+        <v>876</v>
       </c>
       <c r="C181" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D181" s="3">
-        <v>1122</v>
+        <v>876</v>
       </c>
       <c r="E181" s="6">
-        <v>44861.716111111113</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F181" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A182" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B182" s="15">
-        <v>1885</v>
-      </c>
-      <c r="C182" s="16">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D182" s="15">
-        <v>1932</v>
-      </c>
-      <c r="E182" s="16">
-        <v>44852.752916666665</v>
-      </c>
-      <c r="F182" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H182" s="15" t="s">
-        <v>107</v>
+    <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A182" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B182" s="3">
+        <v>571</v>
+      </c>
+      <c r="C182" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D182" s="3">
+        <v>571</v>
+      </c>
+      <c r="E182" s="6">
+        <v>44076.622754629629</v>
+      </c>
+      <c r="F182" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A183" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B183" s="3">
-        <v>1328</v>
+        <v>1122</v>
       </c>
       <c r="C183" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D183" s="3">
+        <v>1122</v>
+      </c>
+      <c r="E183" s="6">
+        <v>44861.716111111113</v>
+      </c>
+      <c r="F183" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A184" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B184" s="15">
+        <v>1885</v>
+      </c>
+      <c r="C184" s="16">
         <v>45533.322094907409</v>
       </c>
-      <c r="D183" s="3">
-        <v>1328</v>
-      </c>
-      <c r="E183" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F183" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A184" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B184" s="3">
-        <v>318</v>
-      </c>
-      <c r="C184" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D184" s="3">
-        <v>318</v>
-      </c>
-      <c r="E184" s="6">
-        <v>42990.77134259259</v>
-      </c>
-      <c r="F184" s="11" t="s">
-        <v>11</v>
+      <c r="D184" s="15">
+        <v>1932</v>
+      </c>
+      <c r="E184" s="16">
+        <v>44852.752916666665</v>
+      </c>
+      <c r="F184" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H184" s="15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A185" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B185" s="3">
-        <v>1009</v>
+        <v>1328</v>
       </c>
       <c r="C185" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D185" s="3">
-        <v>1009</v>
+        <v>1328</v>
       </c>
       <c r="E185" s="6">
-        <v>44852.670138888891</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F185" s="11" t="s">
         <v>11</v>
@@ -6357,19 +6364,19 @@
     </row>
     <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A186" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B186" s="3">
-        <v>1657</v>
+        <v>318</v>
       </c>
       <c r="C186" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D186" s="3">
-        <v>1657</v>
+        <v>318</v>
       </c>
       <c r="E186" s="6">
-        <v>42990.765023148146</v>
+        <v>42990.77134259259</v>
       </c>
       <c r="F186" s="11" t="s">
         <v>11</v>
@@ -6377,209 +6384,209 @@
     </row>
     <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A187" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B187" s="3">
-        <v>1677</v>
+        <v>1009</v>
       </c>
       <c r="C187" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D187" s="3">
-        <v>1677</v>
+        <v>1009</v>
       </c>
       <c r="E187" s="6">
-        <v>44848.55972222222</v>
+        <v>44852.670138888891</v>
       </c>
       <c r="F187" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A188" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B188" s="13">
-        <v>2576</v>
-      </c>
-      <c r="C188" s="14">
+    <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A188" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B188" s="3">
+        <v>1657</v>
+      </c>
+      <c r="C188" s="6">
         <v>45533.322094907409</v>
       </c>
-      <c r="D188" s="13">
-        <v>2576</v>
-      </c>
-      <c r="E188" s="14">
-        <v>43304.752638888887</v>
-      </c>
-      <c r="F188" s="13" t="s">
-        <v>110</v>
+      <c r="D188" s="3">
+        <v>1657</v>
+      </c>
+      <c r="E188" s="6">
+        <v>42990.765023148146</v>
+      </c>
+      <c r="F188" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A189" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B189" s="3">
-        <v>1237</v>
+        <v>1677</v>
       </c>
       <c r="C189" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D189" s="3">
+        <v>1677</v>
+      </c>
+      <c r="E189" s="6">
+        <v>44848.55972222222</v>
+      </c>
+      <c r="F189" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A190" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B190" s="13">
+        <v>2576</v>
+      </c>
+      <c r="C190" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D189" s="3">
-        <v>1237</v>
-      </c>
-      <c r="E189" s="6">
-        <v>43710.58252314815</v>
-      </c>
-      <c r="F189" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A190" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B190" s="3">
-        <v>872</v>
-      </c>
-      <c r="C190" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D190" s="3">
-        <v>872</v>
-      </c>
-      <c r="E190" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F190" s="11" t="s">
-        <v>11</v>
+      <c r="D190" s="13">
+        <v>2576</v>
+      </c>
+      <c r="E190" s="14">
+        <v>43304.752638888887</v>
+      </c>
+      <c r="F190" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="191" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A191" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B191" s="3">
-        <v>2471</v>
+        <v>1237</v>
       </c>
       <c r="C191" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D191" s="3">
+        <v>1237</v>
+      </c>
+      <c r="E191" s="6">
+        <v>43710.58252314815</v>
+      </c>
+      <c r="F191" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A192" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B192" s="3">
+        <v>872</v>
+      </c>
+      <c r="C192" s="6">
+        <v>45533.322094907409</v>
+      </c>
+      <c r="D192" s="3">
+        <v>872</v>
+      </c>
+      <c r="E192" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F192" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A193" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B193" s="3">
         <v>2471</v>
       </c>
-      <c r="E191" s="6">
+      <c r="C193" s="6">
+        <v>45533.322094907409</v>
+      </c>
+      <c r="D193" s="3">
+        <v>2471</v>
+      </c>
+      <c r="E193" s="6">
         <v>42949.567870370367</v>
       </c>
-      <c r="F191" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A192" s="28" t="s">
+      <c r="F193" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A194" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="B192" s="3"/>
-      <c r="C192" s="6"/>
-      <c r="D192" s="3"/>
-      <c r="E192" s="6"/>
-      <c r="F192" s="11"/>
-    </row>
-    <row r="193" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A193" s="13" t="s">
+      <c r="B194" s="3"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="11"/>
+    </row>
+    <row r="195" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A195" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B193" s="13">
+      <c r="B195" s="13">
         <v>492</v>
       </c>
-      <c r="C193" s="14">
+      <c r="C195" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D193" s="13">
+      <c r="D195" s="13">
         <v>492</v>
       </c>
-      <c r="E193" s="14">
+      <c r="E195" s="14">
         <v>44868.679872685185</v>
       </c>
-      <c r="F193" s="13" t="s">
+      <c r="F195" s="13" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A194" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B194" s="3">
-        <v>1135</v>
-      </c>
-      <c r="C194" s="6">
-        <v>45637.672824074078</v>
-      </c>
-      <c r="D194" s="3">
-        <v>1267</v>
-      </c>
-      <c r="E194" s="6">
-        <v>44869.576215277775</v>
-      </c>
-      <c r="F194" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A195" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B195" s="3">
-        <v>3316</v>
-      </c>
-      <c r="C195" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D195" s="3">
-        <v>3316</v>
-      </c>
-      <c r="E195" s="6">
-        <v>44869.449074074073</v>
-      </c>
-      <c r="F195" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A196" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B196" s="3">
-        <v>2293</v>
+        <v>1135</v>
       </c>
       <c r="C196" s="6">
-        <v>45533.322106481479</v>
+        <v>45637.672824074078</v>
       </c>
       <c r="D196" s="3">
-        <v>2293</v>
+        <v>1267</v>
       </c>
       <c r="E196" s="6">
-        <v>44869.446643518517</v>
+        <v>44869.576215277775</v>
       </c>
       <c r="F196" s="11" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A197" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B197" s="3">
-        <v>2288</v>
+        <v>3316</v>
       </c>
       <c r="C197" s="6">
-        <v>45533.322106481479</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D197" s="3">
-        <v>2288</v>
+        <v>3316</v>
       </c>
       <c r="E197" s="6">
-        <v>42949.567847222221</v>
+        <v>44869.449074074073</v>
       </c>
       <c r="F197" s="11" t="s">
         <v>11</v>
@@ -6587,202 +6594,202 @@
     </row>
     <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A198" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B198" s="3">
-        <v>364</v>
+        <v>2293</v>
       </c>
       <c r="C198" s="6">
         <v>45533.322106481479</v>
       </c>
       <c r="D198" s="3">
+        <v>2293</v>
+      </c>
+      <c r="E198" s="6">
+        <v>44869.446643518517</v>
+      </c>
+      <c r="F198" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A199" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B199" s="3">
+        <v>2288</v>
+      </c>
+      <c r="C199" s="6">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D199" s="3">
+        <v>2288</v>
+      </c>
+      <c r="E199" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F199" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A200" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B200" s="3">
         <v>364</v>
       </c>
-      <c r="E198" s="6">
+      <c r="C200" s="6">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D200" s="3">
+        <v>364</v>
+      </c>
+      <c r="E200" s="6">
         <v>43863.785486111112</v>
       </c>
-      <c r="F198" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A199" s="28" t="s">
+      <c r="F200" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A201" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="B199" s="3"/>
-      <c r="C199" s="6"/>
-      <c r="D199" s="3"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="11"/>
-    </row>
-    <row r="200" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="22" t="s">
+      <c r="B201" s="3"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="11"/>
+    </row>
+    <row r="202" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A202" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B200" s="22">
+      <c r="B202" s="22">
         <v>4763</v>
       </c>
-      <c r="C200" s="23">
+      <c r="C202" s="23">
         <v>45622.614722222221</v>
       </c>
-      <c r="D200" s="22">
+      <c r="D202" s="22">
         <v>4832</v>
       </c>
-      <c r="E200" s="23">
+      <c r="E202" s="23">
         <v>44869.413148148145</v>
       </c>
-      <c r="F200" s="22" t="s">
+      <c r="F202" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="H200" s="22" t="s">
+      <c r="H202" s="22" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B201" s="13">
-        <v>483</v>
-      </c>
-      <c r="C201" s="14">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D201" s="13">
-        <v>483</v>
-      </c>
-      <c r="E201" s="14">
-        <v>42992.768796296295</v>
-      </c>
-      <c r="F201" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A202" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B202" s="13">
-        <v>743</v>
-      </c>
-      <c r="C202" s="14">
-        <v>45637.479016203702</v>
-      </c>
-      <c r="D202" s="13">
-        <v>836</v>
-      </c>
-      <c r="E202" s="14">
-        <v>44869.403402777774</v>
-      </c>
-      <c r="F202" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="203" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A203" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B203" s="13">
-        <v>749</v>
+        <v>483</v>
       </c>
       <c r="C203" s="14">
-        <v>45637.479409722226</v>
+        <v>45533.322106481479</v>
       </c>
       <c r="D203" s="13">
-        <v>761</v>
+        <v>483</v>
       </c>
       <c r="E203" s="14">
-        <v>44869.396956018521</v>
+        <v>42992.768796296295</v>
       </c>
       <c r="F203" s="13" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A204" s="13" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="B204" s="13">
-        <v>451</v>
+        <v>743</v>
       </c>
       <c r="C204" s="14">
-        <v>45637.539085648146</v>
+        <v>45637.479016203702</v>
       </c>
       <c r="D204" s="13">
-        <v>401</v>
+        <v>836</v>
       </c>
       <c r="E204" s="14">
-        <v>42999.700740740744</v>
+        <v>44869.403402777774</v>
       </c>
       <c r="F204" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A205" s="28" t="s">
+    <row r="205" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A205" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B205" s="13">
+        <v>749</v>
+      </c>
+      <c r="C205" s="14">
+        <v>45637.479409722226</v>
+      </c>
+      <c r="D205" s="13">
+        <v>761</v>
+      </c>
+      <c r="E205" s="14">
+        <v>44869.396956018521</v>
+      </c>
+      <c r="F205" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A206" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B206" s="13">
+        <v>451</v>
+      </c>
+      <c r="C206" s="14">
+        <v>45637.539085648146</v>
+      </c>
+      <c r="D206" s="13">
+        <v>401</v>
+      </c>
+      <c r="E206" s="14">
+        <v>42999.700740740744</v>
+      </c>
+      <c r="F206" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A207" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B205" s="3"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="3"/>
-      <c r="E205" s="6"/>
-      <c r="F205" s="11"/>
-    </row>
-    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A206" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B206" s="3">
-        <v>815</v>
-      </c>
-      <c r="C206" s="6">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D206" s="3">
-        <v>815</v>
-      </c>
-      <c r="E206" s="6">
-        <v>44865.586435185185</v>
-      </c>
-      <c r="F206" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A207" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B207" s="3">
-        <v>2674</v>
-      </c>
-      <c r="C207" s="6">
-        <v>45637.463252314818</v>
-      </c>
-      <c r="D207" s="3">
-        <v>2649</v>
-      </c>
-      <c r="E207" s="6">
-        <v>44869.507557870369</v>
-      </c>
-      <c r="F207" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="B207" s="3"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="6"/>
+      <c r="F207" s="11"/>
     </row>
     <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A208" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B208" s="3">
-        <v>162</v>
+        <v>815</v>
       </c>
       <c r="C208" s="6">
-        <v>45533.322118055556</v>
+        <v>45533.322106481479</v>
       </c>
       <c r="D208" s="3">
-        <v>162</v>
+        <v>815</v>
       </c>
       <c r="E208" s="6">
-        <v>42949.567870370367</v>
+        <v>44865.586435185185</v>
       </c>
       <c r="F208" s="11" t="s">
         <v>11</v>
@@ -6790,39 +6797,39 @@
     </row>
     <row r="209" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A209" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B209" s="3">
-        <v>286</v>
+        <v>2674</v>
       </c>
       <c r="C209" s="6">
-        <v>45533.322118055556</v>
+        <v>45637.463252314818</v>
       </c>
       <c r="D209" s="3">
-        <v>286</v>
+        <v>2649</v>
       </c>
       <c r="E209" s="6">
-        <v>44861.727037037039</v>
+        <v>44869.507557870369</v>
       </c>
       <c r="F209" s="11" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A210" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B210" s="3">
-        <v>255</v>
+        <v>162</v>
       </c>
       <c r="C210" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D210" s="3">
-        <v>255</v>
+        <v>162</v>
       </c>
       <c r="E210" s="6">
-        <v>44861.727152777778</v>
+        <v>42949.567870370367</v>
       </c>
       <c r="F210" s="11" t="s">
         <v>11</v>
@@ -6830,19 +6837,19 @@
     </row>
     <row r="211" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A211" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B211" s="3">
-        <v>420</v>
+        <v>286</v>
       </c>
       <c r="C211" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D211" s="3">
-        <v>420</v>
+        <v>286</v>
       </c>
       <c r="E211" s="6">
-        <v>44861.727546296293</v>
+        <v>44861.727037037039</v>
       </c>
       <c r="F211" s="11" t="s">
         <v>11</v>
@@ -6850,41 +6857,81 @@
     </row>
     <row r="212" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A212" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B212" s="3">
-        <v>138</v>
+        <v>255</v>
       </c>
       <c r="C212" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D212" s="3">
+        <v>255</v>
+      </c>
+      <c r="E212" s="6">
+        <v>44861.727152777778</v>
+      </c>
+      <c r="F212" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A213" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B213" s="3">
+        <v>420</v>
+      </c>
+      <c r="C213" s="6">
+        <v>45533.322118055556</v>
+      </c>
+      <c r="D213" s="3">
+        <v>420</v>
+      </c>
+      <c r="E213" s="6">
+        <v>44861.727546296293</v>
+      </c>
+      <c r="F213" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A214" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B214" s="3">
         <v>138</v>
       </c>
-      <c r="E212" s="6">
+      <c r="C214" s="6">
+        <v>45533.322118055556</v>
+      </c>
+      <c r="D214" s="3">
+        <v>138</v>
+      </c>
+      <c r="E214" s="6">
         <v>44869.508900462963</v>
       </c>
-      <c r="F212" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A213" s="22" t="s">
+      <c r="F214" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A215" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="B213" s="22">
+      <c r="B215" s="22">
         <v>11219</v>
       </c>
-      <c r="C213" s="23">
+      <c r="C215" s="23">
         <v>45636.606886574074</v>
       </c>
-      <c r="D213" s="22">
+      <c r="D215" s="22">
         <v>13055</v>
       </c>
-      <c r="E213" s="23">
+      <c r="E215" s="23">
         <v>44869.593541666669</v>
       </c>
-      <c r="F213" s="22" t="s">
+      <c r="F215" s="22" t="s">
         <v>55</v>
       </c>
     </row>
@@ -6917,12 +6964,12 @@
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="B81:C81"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D108 A109:B110 D109:E110 A111:E111 A112:B116 D112:E116 A117:E123 A124:D124 B125:D125 A126:D126 A127:E148 A150:E213 B149:E149">
+  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D108 A109:B110 D109:E110 A111:E111 A112:B116 D112:E116 A117:E123 A124:D124 B125:D127 A128:D128 A129:E150 B151:E151 A152:E215">
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="/.">
       <formula>NOT(ISERROR(SEARCH("/.",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 A77:E124 B125:E125 A126:E148 A214:XFD1048576 G77:XFD160 G162:XFD213 G161 I161:XFD161 A150:E213 B149:E149">
+  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 A77:E124 G77:XFD162 B125:E127 A128:E150 B151:E151 A152:E215 G163 I163:XFD163 G164:XFD215 A216:XFD1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
@@ -6937,14 +6984,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D167F10C-888A-4DD5-9D21-B37C2E0CD56C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additional  fixings to setupChannel; redundant UV_LED functions are deleted
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukhina\Documents\MATLAB\ScopeScript-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A01384-1E58-4F48-AA55-2DADBFB70571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CAA528-567E-40E7-A907-0FD40E1A8239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{64517161-2A91-2B47-8856-8DF463AC8E32}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Arduino code check list" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$211</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="248">
   <si>
     <r>
       <t>Left file list</t>
@@ -1782,9 +1782,6 @@
     <t>Laser</t>
   </si>
   <si>
-    <t>LEDs</t>
-  </si>
-  <si>
     <t>PSF</t>
   </si>
   <si>
@@ -1830,12 +1827,6 @@
     <t>hardwareControl/light_sources/printAvailableChannels.m  (open)</t>
   </si>
   <si>
-    <t>hardwareControl/light_sources/leds/BF_LED/turnOFFBFLED.m  (open)</t>
-  </si>
-  <si>
-    <t>hardwareControl/light_sources/leds/BF_LED/turnONBFLED.m  (open)</t>
-  </si>
-  <si>
     <t>printlaserProperties</t>
   </si>
   <si>
@@ -1936,18 +1927,6 @@
   </si>
   <si>
     <t xml:space="preserve"> +/- check with TTL triggering - what mmc.setProperty('UV LED','UV340') does?</t>
-  </si>
-  <si>
-    <t>hardwareControl/light_sources/leds/UV_LED/turnOnUV340.m  (open)</t>
-  </si>
-  <si>
-    <t>hardwareControl/light_sources/leds/UV_LED/turnOnUV380.m  (open)</t>
-  </si>
-  <si>
-    <t>hardwareControl/light_sources/leds/UV_LED/setUV340Intensity.m  (open)</t>
-  </si>
-  <si>
-    <t>hardwareControl/light_sources/leds/UV_LED/setUV380Intensity.m  (open)</t>
   </si>
   <si>
     <t>hardwareControl/light_sources/laser/turnOnAllLasers.m  (open: left | right)</t>
@@ -2233,6 +2212,18 @@
   </si>
   <si>
     <t>getMirrorPosition()</t>
+  </si>
+  <si>
+    <t>BF-LED</t>
+  </si>
+  <si>
+    <t>hardwareControl/light_sources/BF_LED/turnOFFBFLED.m  (open)</t>
+  </si>
+  <si>
+    <t>hardwareControl/light_sources/BF_LED/turnONBFLED.m  (open)</t>
+  </si>
+  <si>
+    <t>redundant? Check for dependencies other than in setupChannel</t>
   </si>
 </sst>
 </file>
@@ -2544,16 +2535,16 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2921,11 +2912,11 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:H215"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125:XFD125"/>
+      <pane ySplit="8" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2966,14 +2957,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
@@ -3011,12 +3002,12 @@
     </row>
     <row r="10" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="37"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="22">
         <v>835</v>
       </c>
@@ -3032,12 +3023,12 @@
     </row>
     <row r="11" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="22">
         <v>2953</v>
       </c>
@@ -3053,12 +3044,12 @@
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="22">
         <v>406</v>
       </c>
@@ -3074,12 +3065,12 @@
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="B13" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="22">
         <v>5488</v>
       </c>
@@ -3095,12 +3086,12 @@
     </row>
     <row r="14" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="22">
         <v>634</v>
       </c>
@@ -3116,12 +3107,12 @@
     </row>
     <row r="15" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="22">
         <v>510</v>
       </c>
@@ -3137,12 +3128,12 @@
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="B16" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="22">
         <v>771</v>
       </c>
@@ -3158,12 +3149,12 @@
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="22">
         <v>1203</v>
       </c>
@@ -3179,12 +3170,12 @@
     </row>
     <row r="18" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="22">
         <v>594</v>
       </c>
@@ -3200,12 +3191,12 @@
     </row>
     <row r="19" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B19" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="37"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="22">
         <v>962</v>
       </c>
@@ -3221,12 +3212,12 @@
     </row>
     <row r="20" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="B20" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="22">
         <v>1255</v>
       </c>
@@ -3242,12 +3233,12 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B21" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="22">
         <v>2288</v>
       </c>
@@ -3263,12 +3254,12 @@
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="22">
         <v>1552</v>
       </c>
@@ -3284,12 +3275,12 @@
     </row>
     <row r="23" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="B23" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="22">
         <v>764</v>
       </c>
@@ -3305,12 +3296,12 @@
     </row>
     <row r="24" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="B24" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="22">
         <v>342</v>
       </c>
@@ -3360,7 +3351,7 @@
     </row>
     <row r="27" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B27" s="22">
         <v>1555</v>
@@ -3378,12 +3369,12 @@
         <v>11</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B28" s="22">
         <v>1477</v>
@@ -3401,12 +3392,12 @@
         <v>11</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B29" s="22">
         <v>197</v>
@@ -3424,12 +3415,12 @@
         <v>11</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B30" s="22">
         <v>1111</v>
@@ -3447,12 +3438,12 @@
         <v>11</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B31" s="22">
         <v>1235</v>
@@ -3470,12 +3461,12 @@
         <v>11</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B32" s="22">
         <v>755</v>
@@ -3493,12 +3484,12 @@
         <v>11</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B33" s="22">
         <v>342</v>
@@ -3516,12 +3507,12 @@
         <v>11</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B34" s="22">
         <v>169</v>
@@ -3539,12 +3530,12 @@
         <v>11</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B35" s="22">
         <v>237</v>
@@ -3562,12 +3553,12 @@
         <v>11</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B36" s="22">
         <v>432</v>
@@ -3585,12 +3576,12 @@
         <v>11</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B37" s="22">
         <v>3069</v>
@@ -3608,12 +3599,12 @@
         <v>11</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B38" s="22">
         <v>303</v>
@@ -3631,12 +3622,12 @@
         <v>11</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B39" s="22">
         <v>698</v>
@@ -3654,12 +3645,12 @@
         <v>11</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B40" s="22">
         <v>605</v>
@@ -3677,12 +3668,12 @@
         <v>11</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B41" s="22">
         <v>988</v>
@@ -3700,12 +3691,12 @@
         <v>11</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B42" s="22">
         <v>387</v>
@@ -3723,12 +3714,12 @@
         <v>11</v>
       </c>
       <c r="H42" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B43" s="22">
         <v>5585</v>
@@ -3746,12 +3737,12 @@
         <v>11</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B44" s="22">
         <v>2983</v>
@@ -3769,12 +3760,12 @@
         <v>110</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B45" s="22">
         <v>1103</v>
@@ -3792,12 +3783,12 @@
         <v>11</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B46" s="22">
         <v>381</v>
@@ -3815,12 +3806,12 @@
         <v>11</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B47" s="22">
         <v>674</v>
@@ -3838,12 +3829,12 @@
         <v>11</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B48" s="22">
         <v>1481</v>
@@ -3861,12 +3852,12 @@
         <v>11</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="22" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B49" s="22">
         <v>1078</v>
@@ -3884,12 +3875,12 @@
         <v>11</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B50" s="22">
         <v>833</v>
@@ -3907,12 +3898,12 @@
         <v>11</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B51" s="22">
         <v>817</v>
@@ -3930,12 +3921,12 @@
         <v>11</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B52" s="22">
         <v>188</v>
@@ -3953,12 +3944,12 @@
         <v>11</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B53" s="22">
         <v>221</v>
@@ -3976,7 +3967,7 @@
         <v>11</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="20" x14ac:dyDescent="0.4">
@@ -4231,10 +4222,10 @@
       <c r="A67" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="34"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="17">
         <v>314</v>
       </c>
@@ -4249,10 +4240,10 @@
       <c r="A68" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="34" t="s">
+      <c r="B68" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="34"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="17">
         <v>308</v>
       </c>
@@ -4372,10 +4363,10 @@
       <c r="A75" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="34" t="s">
+      <c r="B75" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="34"/>
+      <c r="C75" s="36"/>
       <c r="D75" s="17">
         <v>286</v>
       </c>
@@ -4413,10 +4404,10 @@
       <c r="A77" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="36"/>
+      <c r="C77" s="38"/>
       <c r="D77" s="7">
         <v>833</v>
       </c>
@@ -4487,17 +4478,17 @@
         <v>9</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="36"/>
+      <c r="C81" s="38"/>
       <c r="D81" s="7">
         <v>2626</v>
       </c>
@@ -4618,7 +4609,7 @@
     </row>
     <row r="88" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B88" s="13">
         <v>304</v>
@@ -4635,7 +4626,7 @@
     </row>
     <row r="89" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B89" s="13">
         <v>3565</v>
@@ -4652,7 +4643,7 @@
     </row>
     <row r="90" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B90" s="13">
         <v>102</v>
@@ -4670,12 +4661,12 @@
         <v>55</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="20" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B91" s="20">
         <v>159</v>
@@ -4693,12 +4684,12 @@
         <v>10</v>
       </c>
       <c r="H91" s="20" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C92" s="14"/>
       <c r="E92" s="14"/>
@@ -4719,10 +4710,10 @@
       <c r="A94" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="35"/>
+      <c r="C94" s="37"/>
       <c r="D94" s="17">
         <v>709</v>
       </c>
@@ -4735,7 +4726,7 @@
     </row>
     <row r="95" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B95" s="20">
         <v>155</v>
@@ -4755,7 +4746,7 @@
     </row>
     <row r="96" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="20" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B96" s="20">
         <v>1545</v>
@@ -4775,7 +4766,7 @@
     </row>
     <row r="97" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B97" s="20">
         <v>136</v>
@@ -4795,7 +4786,7 @@
     </row>
     <row r="98" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B98" s="20">
         <v>109</v>
@@ -4813,12 +4804,12 @@
         <v>10</v>
       </c>
       <c r="H98" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A99" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C99" s="16"/>
       <c r="E99" s="16"/>
@@ -4826,12 +4817,12 @@
         <v>9</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" s="15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C100" s="16"/>
       <c r="E100" s="16"/>
@@ -4839,12 +4830,12 @@
         <v>9</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" s="15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C101" s="16"/>
       <c r="E101" s="16"/>
@@ -4852,12 +4843,12 @@
         <v>9</v>
       </c>
       <c r="H101" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A102" s="28" t="s">
-        <v>131</v>
+        <v>244</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="6"/>
@@ -4867,7 +4858,7 @@
     </row>
     <row r="103" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A103" s="13" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="B103" s="13">
         <v>196</v>
@@ -4882,248 +4873,251 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B104" s="13">
+    <row r="104" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B104" s="15">
         <v>394</v>
       </c>
-      <c r="C104" s="14">
+      <c r="C104" s="16">
         <v>45639.660196759258</v>
       </c>
-      <c r="D104" s="13" t="s">
+      <c r="D104" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F104" s="13" t="s">
+      <c r="F104" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B105" s="15">
-        <v>266</v>
-      </c>
-      <c r="C105" s="16">
-        <v>45636.49359953704</v>
-      </c>
-      <c r="D105" s="15" t="s">
+      <c r="H104" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A105" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B105" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F105" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H105" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B106" s="15">
-        <v>266</v>
-      </c>
-      <c r="C106" s="16">
-        <v>45636.493784722225</v>
-      </c>
-      <c r="D106" s="15" t="s">
+      <c r="D105" s="17">
+        <v>262</v>
+      </c>
+      <c r="E105" s="18">
+        <v>42962.894861111112</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F106" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H106" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B107" s="15">
+      <c r="D106" s="20">
+        <v>464</v>
+      </c>
+      <c r="E106" s="20">
+        <v>44862.503541666665</v>
+      </c>
+      <c r="F106" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A107" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="17">
+        <v>4585</v>
+      </c>
+      <c r="C107" s="18">
+        <v>45533.321979166663</v>
+      </c>
+      <c r="D107" s="17">
+        <v>4585</v>
+      </c>
+      <c r="E107" s="18">
+        <v>44390.836111111108</v>
+      </c>
+      <c r="F107" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="35"/>
+      <c r="D108" s="20">
+        <v>1225</v>
+      </c>
+      <c r="E108" s="20">
+        <v>44862.499490740738</v>
+      </c>
+      <c r="F108" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="35"/>
+      <c r="D109" s="20">
+        <v>1053</v>
+      </c>
+      <c r="E109" s="20">
+        <v>44862.498703703706</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A110" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="36"/>
+      <c r="D110" s="17">
+        <v>6709</v>
+      </c>
+      <c r="E110" s="18">
+        <v>44868.709155092591</v>
+      </c>
+      <c r="F110" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" s="20">
+        <v>285</v>
+      </c>
+      <c r="E111" s="20">
+        <v>44846.595578703702</v>
+      </c>
+      <c r="F111" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A112" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C107" s="16">
-        <v>45639.66684027778</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F107" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B108" s="15">
-        <v>91</v>
-      </c>
-      <c r="C108" s="16">
-        <v>45639.667962962965</v>
-      </c>
-      <c r="D108" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F108" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H108" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A109" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B109" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D109" s="17">
-        <v>262</v>
-      </c>
-      <c r="E109" s="18">
-        <v>42962.894861111112</v>
-      </c>
-      <c r="F109" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B110" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D110" s="20">
-        <v>464</v>
-      </c>
-      <c r="E110" s="20">
-        <v>44862.503541666665</v>
-      </c>
-      <c r="F110" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A111" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B111" s="17">
-        <v>4585</v>
-      </c>
-      <c r="C111" s="18">
-        <v>45533.321979166663</v>
-      </c>
-      <c r="D111" s="17">
-        <v>4585</v>
-      </c>
-      <c r="E111" s="18">
-        <v>44390.836111111108</v>
-      </c>
-      <c r="F111" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B112" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C112" s="33"/>
-      <c r="D112" s="20">
-        <v>1225</v>
-      </c>
-      <c r="E112" s="20">
-        <v>44862.499490740738</v>
-      </c>
-      <c r="F112" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C113" s="33"/>
-      <c r="D113" s="20">
-        <v>1053</v>
-      </c>
-      <c r="E113" s="20">
-        <v>44862.498703703706</v>
-      </c>
-      <c r="F113" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A114" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B114" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C114" s="34"/>
-      <c r="D114" s="17">
-        <v>6709</v>
-      </c>
-      <c r="E114" s="18">
-        <v>44868.709155092591</v>
-      </c>
-      <c r="F114" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B115" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D115" s="20">
-        <v>285</v>
-      </c>
-      <c r="E115" s="20">
-        <v>44846.595578703702</v>
-      </c>
-      <c r="F115" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A116" s="27" t="s">
-        <v>132</v>
+      <c r="B113" s="13">
+        <v>316</v>
+      </c>
+      <c r="C113" s="14">
+        <v>45533.322002314817</v>
+      </c>
+      <c r="D113" s="13">
+        <v>316</v>
+      </c>
+      <c r="E113" s="14">
+        <v>42977.691412037035</v>
+      </c>
+      <c r="F113" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B114" s="13">
+        <v>345</v>
+      </c>
+      <c r="C114" s="14">
+        <v>45533.322002314817</v>
+      </c>
+      <c r="D114" s="13">
+        <v>345</v>
+      </c>
+      <c r="E114" s="14">
+        <v>44852.729004629633</v>
+      </c>
+      <c r="F114" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B115" s="13">
+        <v>264</v>
+      </c>
+      <c r="C115" s="14">
+        <v>45533.322002314817</v>
+      </c>
+      <c r="D115" s="13">
+        <v>264</v>
+      </c>
+      <c r="E115" s="14">
+        <v>44852.731087962966</v>
+      </c>
+      <c r="F115" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B116" s="13">
+        <v>223</v>
+      </c>
+      <c r="C116" s="14">
+        <v>45533.322002314817</v>
+      </c>
+      <c r="D116" s="13">
+        <v>223</v>
+      </c>
+      <c r="E116" s="14">
+        <v>44865.57439814815</v>
+      </c>
+      <c r="F116" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B117" s="13">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="C117" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D117" s="13">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="E117" s="14">
-        <v>42977.691412037035</v>
+        <v>44865.574004629627</v>
       </c>
       <c r="F117" s="13" t="s">
         <v>11</v>
@@ -5131,177 +5125,177 @@
     </row>
     <row r="118" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B118" s="13">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="C118" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D118" s="13">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E118" s="14">
-        <v>44852.729004629633</v>
+        <v>44865.573680555557</v>
       </c>
       <c r="F118" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A119" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B119" s="13">
-        <v>264</v>
-      </c>
-      <c r="C119" s="14">
+    <row r="119" spans="1:6" ht="23.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A119" s="27" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A120" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B120" s="22">
+        <v>199</v>
+      </c>
+      <c r="C120" s="23">
+        <v>45638.596597222226</v>
+      </c>
+      <c r="D120" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A121" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C121" s="14"/>
+      <c r="F121" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A122" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C122" s="14"/>
+      <c r="F122" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C123" s="14"/>
+      <c r="F123" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+      <c r="A124" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="5"/>
+      <c r="F124" s="11"/>
+    </row>
+    <row r="125" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B125" s="13">
+        <v>257</v>
+      </c>
+      <c r="C125" s="14">
         <v>45533.322002314817</v>
       </c>
-      <c r="D119" s="13">
-        <v>264</v>
-      </c>
-      <c r="E119" s="14">
-        <v>44852.731087962966</v>
-      </c>
-      <c r="F119" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A120" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B120" s="13">
-        <v>223</v>
-      </c>
-      <c r="C120" s="14">
+      <c r="D125" s="13">
+        <v>257</v>
+      </c>
+      <c r="E125" s="14">
+        <v>42978.469814814816</v>
+      </c>
+      <c r="F125" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B126" s="13">
+        <v>536</v>
+      </c>
+      <c r="C126" s="14">
         <v>45533.322002314817</v>
       </c>
-      <c r="D120" s="13">
-        <v>223</v>
-      </c>
-      <c r="E120" s="14">
-        <v>44865.57439814815</v>
-      </c>
-      <c r="F120" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A121" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B121" s="13">
-        <v>304</v>
-      </c>
-      <c r="C121" s="14">
+      <c r="D126" s="13">
+        <v>536</v>
+      </c>
+      <c r="E126" s="14">
+        <v>42978.465370370373</v>
+      </c>
+      <c r="F126" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B127" s="13">
+        <v>472</v>
+      </c>
+      <c r="C127" s="14">
         <v>45533.322002314817</v>
       </c>
-      <c r="D121" s="13">
-        <v>304</v>
-      </c>
-      <c r="E121" s="14">
-        <v>44865.574004629627</v>
-      </c>
-      <c r="F121" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A122" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B122" s="13">
-        <v>1449</v>
-      </c>
-      <c r="C122" s="14">
+      <c r="D127" s="13">
+        <v>472</v>
+      </c>
+      <c r="E127" s="14">
+        <v>43041.741759259261</v>
+      </c>
+      <c r="F127" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B128" s="13">
+        <v>257</v>
+      </c>
+      <c r="C128" s="14">
         <v>45533.322002314817</v>
       </c>
-      <c r="D122" s="13">
-        <v>1449</v>
-      </c>
-      <c r="E122" s="14">
-        <v>44865.573680555557</v>
-      </c>
-      <c r="F122" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="23.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A123" s="27" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A124" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B124" s="22">
-        <v>199</v>
-      </c>
-      <c r="C124" s="23">
-        <v>45638.596597222226</v>
-      </c>
-      <c r="D124" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F124" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A125" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="C125" s="14"/>
-      <c r="F125" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A126" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="C126" s="14"/>
-      <c r="F126" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A127" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="C127" s="14"/>
-      <c r="F127" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A128" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B128" s="3"/>
-      <c r="C128" s="6"/>
-      <c r="D128" s="5"/>
-      <c r="F128" s="11"/>
+      <c r="D128" s="13">
+        <v>257</v>
+      </c>
+      <c r="E128" s="14">
+        <v>42978.510162037041</v>
+      </c>
+      <c r="F128" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="129" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B129" s="13">
-        <v>257</v>
+        <v>741</v>
       </c>
       <c r="C129" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D129" s="13">
-        <v>257</v>
+        <v>741</v>
       </c>
       <c r="E129" s="14">
-        <v>42978.469814814816</v>
+        <v>42978.451574074075</v>
       </c>
       <c r="F129" s="13" t="s">
         <v>11</v>
@@ -5309,19 +5303,19 @@
     </row>
     <row r="130" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B130" s="13">
-        <v>536</v>
+        <v>112</v>
       </c>
       <c r="C130" s="14">
-        <v>45533.322002314817</v>
+        <v>45533.322013888886</v>
       </c>
       <c r="D130" s="13">
-        <v>536</v>
+        <v>112</v>
       </c>
       <c r="E130" s="14">
-        <v>42978.465370370373</v>
+        <v>44865.577453703707</v>
       </c>
       <c r="F130" s="13" t="s">
         <v>11</v>
@@ -5329,19 +5323,19 @@
     </row>
     <row r="131" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B131" s="13">
-        <v>472</v>
+        <v>77</v>
       </c>
       <c r="C131" s="14">
-        <v>45533.322002314817</v>
+        <v>45533.322013888886</v>
       </c>
       <c r="D131" s="13">
-        <v>472</v>
+        <v>77</v>
       </c>
       <c r="E131" s="14">
-        <v>43041.741759259261</v>
+        <v>42977.54828703704</v>
       </c>
       <c r="F131" s="13" t="s">
         <v>11</v>
@@ -5349,19 +5343,19 @@
     </row>
     <row r="132" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B132" s="13">
-        <v>257</v>
+        <v>125</v>
       </c>
       <c r="C132" s="14">
-        <v>45533.322002314817</v>
+        <v>45533.322013888886</v>
       </c>
       <c r="D132" s="13">
-        <v>257</v>
+        <v>125</v>
       </c>
       <c r="E132" s="14">
-        <v>42978.510162037041</v>
+        <v>42992.41233796296</v>
       </c>
       <c r="F132" s="13" t="s">
         <v>11</v>
@@ -5369,525 +5363,528 @@
     </row>
     <row r="133" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B133" s="13">
-        <v>741</v>
+        <v>310</v>
       </c>
       <c r="C133" s="14">
-        <v>45533.322002314817</v>
+        <v>45533.322013888886</v>
       </c>
       <c r="D133" s="13">
-        <v>741</v>
+        <v>310</v>
       </c>
       <c r="E133" s="14">
-        <v>42978.451574074075</v>
+        <v>44865.57775462963</v>
       </c>
       <c r="F133" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A134" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B134" s="13">
-        <v>112</v>
-      </c>
-      <c r="C134" s="14">
+    <row r="134" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B134" s="15">
+        <v>386</v>
+      </c>
+      <c r="C134" s="16">
         <v>45533.322013888886</v>
       </c>
-      <c r="D134" s="13">
-        <v>112</v>
-      </c>
-      <c r="E134" s="14">
-        <v>44865.577453703707</v>
-      </c>
-      <c r="F134" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A135" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B135" s="13">
-        <v>77</v>
-      </c>
-      <c r="C135" s="14">
+      <c r="D134" s="15">
+        <v>386</v>
+      </c>
+      <c r="E134" s="16">
+        <v>44865.615277777775</v>
+      </c>
+      <c r="F134" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H134" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A135" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B135" s="15">
+        <v>264</v>
+      </c>
+      <c r="C135" s="16">
         <v>45533.322013888886</v>
       </c>
-      <c r="D135" s="13">
-        <v>77</v>
-      </c>
-      <c r="E135" s="14">
-        <v>42977.54828703704</v>
-      </c>
-      <c r="F135" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A136" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B136" s="13">
-        <v>125</v>
-      </c>
-      <c r="C136" s="14">
+      <c r="D135" s="15">
+        <v>264</v>
+      </c>
+      <c r="E135" s="16">
+        <v>42989.788611111115</v>
+      </c>
+      <c r="F135" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H135" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A136" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B136" s="15">
+        <v>232</v>
+      </c>
+      <c r="C136" s="16">
         <v>45533.322013888886</v>
       </c>
-      <c r="D136" s="13">
-        <v>125</v>
-      </c>
-      <c r="E136" s="14">
-        <v>42992.41233796296</v>
-      </c>
-      <c r="F136" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B137" s="13">
-        <v>310</v>
-      </c>
-      <c r="C137" s="14">
+      <c r="D136" s="15">
+        <v>232</v>
+      </c>
+      <c r="E136" s="16">
+        <v>44865.616296296299</v>
+      </c>
+      <c r="F136" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H136" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B137" s="15">
+        <v>284</v>
+      </c>
+      <c r="C137" s="16">
         <v>45533.322013888886</v>
       </c>
-      <c r="D137" s="13">
-        <v>310</v>
-      </c>
-      <c r="E137" s="14">
-        <v>44865.57775462963</v>
-      </c>
-      <c r="F137" s="13" t="s">
-        <v>11</v>
+      <c r="D137" s="15">
+        <v>284</v>
+      </c>
+      <c r="E137" s="16">
+        <v>42989.793263888889</v>
+      </c>
+      <c r="F137" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H137" s="15" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B138" s="15">
-        <v>386</v>
+        <v>1048</v>
       </c>
       <c r="C138" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D138" s="15">
-        <v>386</v>
+        <v>1048</v>
       </c>
       <c r="E138" s="16">
-        <v>44865.615277777775</v>
+        <v>44869.567465277774</v>
       </c>
       <c r="F138" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H138" s="15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B139" s="15">
-        <v>264</v>
+        <v>130</v>
       </c>
       <c r="C139" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D139" s="15">
-        <v>264</v>
+        <v>130</v>
       </c>
       <c r="E139" s="16">
-        <v>42989.788611111115</v>
+        <v>44865.584699074076</v>
       </c>
       <c r="F139" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H139" s="15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B140" s="15">
-        <v>232</v>
+        <v>468</v>
       </c>
       <c r="C140" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D140" s="15">
+        <v>468</v>
+      </c>
+      <c r="E140" s="16">
+        <v>44865.591597222221</v>
+      </c>
+      <c r="F140" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H140" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A141" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A142" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B142" s="22">
+        <v>2387</v>
+      </c>
+      <c r="C142" s="23">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D142" s="22">
+        <v>2387</v>
+      </c>
+      <c r="E142" s="23">
+        <v>44862.525694444441</v>
+      </c>
+      <c r="F142" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B143" s="13">
+        <v>156</v>
+      </c>
+      <c r="C143" s="14">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D143" s="13">
+        <v>156</v>
+      </c>
+      <c r="E143" s="14">
+        <v>42949.567870370367</v>
+      </c>
+      <c r="F143" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A144" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A145" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F145" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H145" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="F146" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H146" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A147" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="E140" s="16">
-        <v>44865.616296296299</v>
-      </c>
-      <c r="F140" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H140" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A141" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B141" s="15">
-        <v>284</v>
-      </c>
-      <c r="C141" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D141" s="15">
-        <v>284</v>
-      </c>
-      <c r="E141" s="16">
-        <v>42989.793263888889</v>
-      </c>
-      <c r="F141" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H141" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A142" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B142" s="15">
-        <v>1048</v>
-      </c>
-      <c r="C142" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D142" s="15">
-        <v>1048</v>
-      </c>
-      <c r="E142" s="16">
-        <v>44869.567465277774</v>
-      </c>
-      <c r="F142" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H142" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A143" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B143" s="15">
-        <v>130</v>
-      </c>
-      <c r="C143" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D143" s="15">
-        <v>130</v>
-      </c>
-      <c r="E143" s="16">
-        <v>44865.584699074076</v>
-      </c>
-      <c r="F143" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H143" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B144" s="15">
-        <v>468</v>
-      </c>
-      <c r="C144" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D144" s="15">
-        <v>468</v>
-      </c>
-      <c r="E144" s="16">
-        <v>44865.591597222221</v>
-      </c>
-      <c r="F144" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H144" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A145" s="27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B146" s="22">
-        <v>2387</v>
-      </c>
-      <c r="C146" s="23">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D146" s="22">
-        <v>2387</v>
-      </c>
-      <c r="E146" s="23">
-        <v>44862.525694444441</v>
-      </c>
-      <c r="F146" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A147" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B147" s="13">
-        <v>156</v>
-      </c>
-      <c r="C147" s="14">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D147" s="13">
-        <v>156</v>
-      </c>
-      <c r="E147" s="14">
-        <v>42949.567870370367</v>
-      </c>
       <c r="F147" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A148" s="27" t="s">
-        <v>135</v>
+        <v>9</v>
+      </c>
+      <c r="H147" s="13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="20">
+        <v>260</v>
+      </c>
+      <c r="C148" s="20">
+        <v>45533.32203703704</v>
+      </c>
+      <c r="D148" s="20">
+        <v>260</v>
+      </c>
+      <c r="E148" s="20">
+        <v>44865.684282407405</v>
+      </c>
+      <c r="F148" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H148" s="20" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A149" s="13" t="s">
-        <v>238</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C149" s="14"/>
+      <c r="E149" s="14"/>
       <c r="F149" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H149" s="13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A150" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="F150" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H150" s="13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="F151" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H151" s="13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A152" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B152" s="20">
-        <v>260</v>
-      </c>
-      <c r="C152" s="20">
+    </row>
+    <row r="150" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B150" s="20">
+        <v>265</v>
+      </c>
+      <c r="C150" s="20">
         <v>45533.32203703704</v>
       </c>
-      <c r="D152" s="20">
-        <v>260</v>
-      </c>
-      <c r="E152" s="20">
-        <v>44865.684282407405</v>
-      </c>
-      <c r="F152" s="20" t="s">
+      <c r="D150" s="20">
+        <v>265</v>
+      </c>
+      <c r="E150" s="20">
+        <v>44868.638414351852</v>
+      </c>
+      <c r="F150" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H152" s="20" t="s">
-        <v>245</v>
+      <c r="H150" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A151" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B151" s="20">
+        <v>275</v>
+      </c>
+      <c r="C151" s="20">
+        <v>45533.32203703704</v>
+      </c>
+      <c r="D151" s="20">
+        <v>275</v>
+      </c>
+      <c r="E151" s="20">
+        <v>44868.639050925929</v>
+      </c>
+      <c r="F151" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H151" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A152" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B152" s="13">
+        <v>1257</v>
+      </c>
+      <c r="C152" s="14">
+        <v>45636.738125000003</v>
+      </c>
+      <c r="D152" s="13">
+        <v>749</v>
+      </c>
+      <c r="E152" s="14">
+        <v>44865.678263888891</v>
+      </c>
+      <c r="F152" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A153" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="C153" s="14"/>
-      <c r="E153" s="14"/>
+        <v>202</v>
+      </c>
+      <c r="B153" s="13">
+        <v>906</v>
+      </c>
+      <c r="C153" s="14">
+        <v>45636.727048611108</v>
+      </c>
+      <c r="D153" s="13">
+        <v>767</v>
+      </c>
+      <c r="E153" s="14">
+        <v>44865.681134259263</v>
+      </c>
       <c r="F153" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A154" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="B154" s="20">
-        <v>265</v>
-      </c>
-      <c r="C154" s="20">
-        <v>45533.32203703704</v>
-      </c>
-      <c r="D154" s="20">
-        <v>265</v>
-      </c>
-      <c r="E154" s="20">
-        <v>44868.638414351852</v>
-      </c>
-      <c r="F154" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H154" s="20" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A155" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B155" s="20">
-        <v>275</v>
-      </c>
-      <c r="C155" s="20">
-        <v>45533.32203703704</v>
-      </c>
-      <c r="D155" s="20">
-        <v>275</v>
-      </c>
-      <c r="E155" s="20">
-        <v>44868.639050925929</v>
-      </c>
-      <c r="F155" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H155" s="20" t="s">
-        <v>235</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A154" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B154" s="15">
+        <v>1057</v>
+      </c>
+      <c r="C154" s="16">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D154" s="15">
+        <v>1057</v>
+      </c>
+      <c r="E154" s="16">
+        <v>44865.684537037036</v>
+      </c>
+      <c r="F154" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H154" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B155" s="13">
+        <v>358</v>
+      </c>
+      <c r="C155" s="14">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D155" s="13">
+        <v>358</v>
+      </c>
+      <c r="E155" s="14">
+        <v>44865.660231481481</v>
+      </c>
+      <c r="F155" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" s="13" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B156" s="13">
-        <v>1257</v>
+        <v>365</v>
       </c>
       <c r="C156" s="14">
-        <v>45636.738125000003</v>
+        <v>45533.322048611109</v>
       </c>
       <c r="D156" s="13">
-        <v>749</v>
+        <v>365</v>
       </c>
       <c r="E156" s="14">
-        <v>44865.678263888891</v>
+        <v>44865.659814814811</v>
       </c>
       <c r="F156" s="13" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="13" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B157" s="13">
-        <v>906</v>
+        <v>563</v>
       </c>
       <c r="C157" s="14">
-        <v>45636.727048611108</v>
+        <v>45533.322048611109</v>
       </c>
       <c r="D157" s="13">
-        <v>767</v>
+        <v>563</v>
       </c>
       <c r="E157" s="14">
-        <v>44865.681134259263</v>
+        <v>44865.672083333331</v>
       </c>
       <c r="F157" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A158" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B158" s="13">
+        <v>253</v>
+      </c>
+      <c r="C158" s="14">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D158" s="13">
+        <v>253</v>
+      </c>
+      <c r="E158" s="14">
+        <v>44865.664467592593</v>
+      </c>
+      <c r="F158" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A159" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="B158" s="15">
-        <v>1057</v>
-      </c>
-      <c r="C158" s="16">
+      <c r="B159" s="22">
+        <v>1062</v>
+      </c>
+      <c r="C159" s="23">
         <v>45533.322048611109</v>
       </c>
-      <c r="D158" s="15">
-        <v>1057</v>
-      </c>
-      <c r="E158" s="16">
-        <v>44865.684537037036</v>
-      </c>
-      <c r="F158" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H158" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A159" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="B159" s="13">
-        <v>358</v>
-      </c>
-      <c r="C159" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D159" s="13">
-        <v>358</v>
-      </c>
-      <c r="E159" s="14">
-        <v>44865.660231481481</v>
-      </c>
-      <c r="F159" s="13" t="s">
-        <v>11</v>
+      <c r="D159" s="22">
+        <v>1062</v>
+      </c>
+      <c r="E159" s="23">
+        <v>44865.663032407407</v>
+      </c>
+      <c r="F159" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H159" s="30" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B160" s="13">
-        <v>365</v>
+        <v>499</v>
       </c>
       <c r="C160" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D160" s="13">
-        <v>365</v>
+        <v>499</v>
       </c>
       <c r="E160" s="14">
-        <v>44865.659814814811</v>
+        <v>44846.595578703702</v>
       </c>
       <c r="F160" s="13" t="s">
         <v>11</v>
@@ -5895,19 +5892,19 @@
     </row>
     <row r="161" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" s="13" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B161" s="13">
-        <v>563</v>
+        <v>285</v>
       </c>
       <c r="C161" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D161" s="13">
-        <v>563</v>
+        <v>285</v>
       </c>
       <c r="E161" s="14">
-        <v>44865.672083333331</v>
+        <v>44846.595578703702</v>
       </c>
       <c r="F161" s="13" t="s">
         <v>11</v>
@@ -5915,159 +5912,156 @@
     </row>
     <row r="162" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B162" s="13">
-        <v>253</v>
+        <v>989</v>
       </c>
       <c r="C162" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D162" s="13">
-        <v>253</v>
+        <v>989</v>
       </c>
       <c r="E162" s="14">
-        <v>44865.664467592593</v>
+        <v>44865.669976851852</v>
       </c>
       <c r="F162" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="B163" s="22">
-        <v>1062</v>
-      </c>
-      <c r="C163" s="23">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D163" s="22">
-        <v>1062</v>
-      </c>
-      <c r="E163" s="23">
-        <v>44865.663032407407</v>
-      </c>
-      <c r="F163" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H163" s="30" t="s">
-        <v>233</v>
-      </c>
+    <row r="163" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A163" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B163" s="3"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="11"/>
     </row>
     <row r="164" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" s="13" t="s">
-        <v>222</v>
+        <v>136</v>
       </c>
       <c r="B164" s="13">
-        <v>499</v>
+        <v>329</v>
       </c>
       <c r="C164" s="14">
-        <v>45533.322048611109</v>
+        <v>45637.51290509259</v>
       </c>
       <c r="D164" s="13">
-        <v>499</v>
+        <v>418</v>
       </c>
       <c r="E164" s="14">
-        <v>44846.595578703702</v>
+        <v>44869.465717592589</v>
       </c>
       <c r="F164" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A165" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B165" s="13">
-        <v>285</v>
-      </c>
-      <c r="C165" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D165" s="13">
-        <v>285</v>
-      </c>
-      <c r="E165" s="14">
-        <v>44846.595578703702</v>
-      </c>
-      <c r="F165" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A166" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B166" s="13">
-        <v>989</v>
-      </c>
-      <c r="C166" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D166" s="13">
-        <v>989</v>
-      </c>
-      <c r="E166" s="14">
-        <v>44865.669976851852</v>
-      </c>
-      <c r="F166" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A167" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B167" s="3"/>
-      <c r="C167" s="6"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="6"/>
-      <c r="F167" s="11"/>
-    </row>
-    <row r="168" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A168" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B168" s="13">
-        <v>329</v>
-      </c>
-      <c r="C168" s="14">
-        <v>45637.51290509259</v>
-      </c>
-      <c r="D168" s="13">
-        <v>418</v>
-      </c>
-      <c r="E168" s="14">
-        <v>44869.465717592589</v>
-      </c>
-      <c r="F168" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A169" s="28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A170" s="28" t="s">
-        <v>143</v>
+    <row r="165" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A165" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A166" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B167" s="3">
+        <v>181</v>
+      </c>
+      <c r="C167" s="6">
+        <v>45533.322071759256</v>
+      </c>
+      <c r="D167" s="3">
+        <v>181</v>
+      </c>
+      <c r="E167" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F167" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B168" s="3">
+        <v>242</v>
+      </c>
+      <c r="C168" s="6">
+        <v>45533.322071759256</v>
+      </c>
+      <c r="D168" s="3">
+        <v>242</v>
+      </c>
+      <c r="E168" s="6">
+        <v>43763.840231481481</v>
+      </c>
+      <c r="F168" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B169" s="3">
+        <v>1778</v>
+      </c>
+      <c r="C169" s="6">
+        <v>45533.322071759256</v>
+      </c>
+      <c r="D169" s="3">
+        <v>1778</v>
+      </c>
+      <c r="E169" s="6">
+        <v>44868.696817129632</v>
+      </c>
+      <c r="F169" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A170" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B170" s="3">
+        <v>1520</v>
+      </c>
+      <c r="C170" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D170" s="3">
+        <v>1520</v>
+      </c>
+      <c r="E170" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A171" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B171" s="3">
-        <v>181</v>
+        <v>791</v>
       </c>
       <c r="C171" s="6">
-        <v>45533.322071759256</v>
+        <v>45533.322083333333</v>
       </c>
       <c r="D171" s="3">
-        <v>181</v>
+        <v>791</v>
       </c>
       <c r="E171" s="6">
         <v>42949.567847222221</v>
@@ -6078,19 +6072,19 @@
     </row>
     <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A172" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B172" s="3">
-        <v>242</v>
+        <v>761</v>
       </c>
       <c r="C172" s="6">
-        <v>45533.322071759256</v>
+        <v>45533.322083333333</v>
       </c>
       <c r="D172" s="3">
-        <v>242</v>
+        <v>761</v>
       </c>
       <c r="E172" s="6">
-        <v>43763.840231481481</v>
+        <v>42990.771851851852</v>
       </c>
       <c r="F172" s="11" t="s">
         <v>11</v>
@@ -6098,19 +6092,19 @@
     </row>
     <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A173" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B173" s="3">
-        <v>1778</v>
+        <v>173</v>
       </c>
       <c r="C173" s="6">
-        <v>45533.322071759256</v>
+        <v>45533.322083333333</v>
       </c>
       <c r="D173" s="3">
-        <v>1778</v>
+        <v>173</v>
       </c>
       <c r="E173" s="6">
-        <v>44868.696817129632</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F173" s="11" t="s">
         <v>11</v>
@@ -6118,59 +6112,62 @@
     </row>
     <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A174" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B174" s="3">
-        <v>1520</v>
+        <v>1710</v>
       </c>
       <c r="C174" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D174" s="3">
-        <v>1520</v>
+        <v>1710</v>
       </c>
       <c r="E174" s="6">
-        <v>42949.567847222221</v>
+        <v>43711.608078703706</v>
       </c>
       <c r="F174" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A175" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B175" s="3">
-        <v>791</v>
-      </c>
-      <c r="C175" s="6">
-        <v>45533.322083333333</v>
-      </c>
-      <c r="D175" s="3">
-        <v>791</v>
-      </c>
-      <c r="E175" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F175" s="11" t="s">
-        <v>11</v>
+    <row r="175" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A175" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B175" s="22">
+        <v>3385</v>
+      </c>
+      <c r="C175" s="23">
+        <v>45637.536157407405</v>
+      </c>
+      <c r="D175" s="22">
+        <v>3379</v>
+      </c>
+      <c r="E175" s="23">
+        <v>44865.695879629631</v>
+      </c>
+      <c r="F175" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H175" s="22" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A176" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B176" s="3">
-        <v>761</v>
+        <v>261</v>
       </c>
       <c r="C176" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D176" s="3">
-        <v>761</v>
+        <v>261</v>
       </c>
       <c r="E176" s="6">
-        <v>42990.771851851852</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F176" s="11" t="s">
         <v>11</v>
@@ -6178,16 +6175,16 @@
     </row>
     <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A177" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B177" s="3">
-        <v>173</v>
+        <v>876</v>
       </c>
       <c r="C177" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D177" s="3">
-        <v>173</v>
+        <v>876</v>
       </c>
       <c r="E177" s="6">
         <v>42949.567847222221</v>
@@ -6198,79 +6195,79 @@
     </row>
     <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A178" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B178" s="3">
-        <v>1710</v>
+        <v>571</v>
       </c>
       <c r="C178" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D178" s="3">
-        <v>1710</v>
+        <v>571</v>
       </c>
       <c r="E178" s="6">
-        <v>43711.608078703706</v>
+        <v>44076.622754629629</v>
       </c>
       <c r="F178" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A179" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B179" s="22">
-        <v>3385</v>
-      </c>
-      <c r="C179" s="23">
-        <v>45637.536157407405</v>
-      </c>
-      <c r="D179" s="22">
-        <v>3379</v>
-      </c>
-      <c r="E179" s="23">
-        <v>44865.695879629631</v>
-      </c>
-      <c r="F179" s="22" t="s">
+    <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A179" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B179" s="3">
+        <v>1122</v>
+      </c>
+      <c r="C179" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D179" s="3">
+        <v>1122</v>
+      </c>
+      <c r="E179" s="6">
+        <v>44861.716111111113</v>
+      </c>
+      <c r="F179" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A180" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B180" s="15">
+        <v>1885</v>
+      </c>
+      <c r="C180" s="16">
+        <v>45533.322094907409</v>
+      </c>
+      <c r="D180" s="15">
+        <v>1932</v>
+      </c>
+      <c r="E180" s="16">
+        <v>44852.752916666665</v>
+      </c>
+      <c r="F180" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H179" s="22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A180" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B180" s="3">
-        <v>261</v>
-      </c>
-      <c r="C180" s="6">
-        <v>45533.322083333333</v>
-      </c>
-      <c r="D180" s="3">
-        <v>261</v>
-      </c>
-      <c r="E180" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F180" s="11" t="s">
-        <v>11</v>
+      <c r="H180" s="15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A181" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B181" s="3">
-        <v>876</v>
+        <v>1328</v>
       </c>
       <c r="C181" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D181" s="3">
-        <v>876</v>
+        <v>1328</v>
       </c>
       <c r="E181" s="6">
         <v>42949.567847222221</v>
@@ -6281,19 +6278,19 @@
     </row>
     <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A182" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B182" s="3">
-        <v>571</v>
+        <v>318</v>
       </c>
       <c r="C182" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D182" s="3">
-        <v>571</v>
+        <v>318</v>
       </c>
       <c r="E182" s="6">
-        <v>44076.622754629629</v>
+        <v>42990.77134259259</v>
       </c>
       <c r="F182" s="11" t="s">
         <v>11</v>
@@ -6301,102 +6298,99 @@
     </row>
     <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A183" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B183" s="3">
-        <v>1122</v>
+        <v>1009</v>
       </c>
       <c r="C183" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D183" s="3">
-        <v>1122</v>
+        <v>1009</v>
       </c>
       <c r="E183" s="6">
-        <v>44861.716111111113</v>
+        <v>44852.670138888891</v>
       </c>
       <c r="F183" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A184" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B184" s="15">
-        <v>1885</v>
-      </c>
-      <c r="C184" s="16">
+    <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A184" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B184" s="3">
+        <v>1657</v>
+      </c>
+      <c r="C184" s="6">
         <v>45533.322094907409</v>
       </c>
-      <c r="D184" s="15">
-        <v>1932</v>
-      </c>
-      <c r="E184" s="16">
-        <v>44852.752916666665</v>
-      </c>
-      <c r="F184" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H184" s="15" t="s">
-        <v>107</v>
+      <c r="D184" s="3">
+        <v>1657</v>
+      </c>
+      <c r="E184" s="6">
+        <v>42990.765023148146</v>
+      </c>
+      <c r="F184" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A185" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B185" s="3">
-        <v>1328</v>
+        <v>1677</v>
       </c>
       <c r="C185" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D185" s="3">
+        <v>1677</v>
+      </c>
+      <c r="E185" s="6">
+        <v>44848.55972222222</v>
+      </c>
+      <c r="F185" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A186" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B186" s="13">
+        <v>2576</v>
+      </c>
+      <c r="C186" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D185" s="3">
-        <v>1328</v>
-      </c>
-      <c r="E185" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F185" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A186" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B186" s="3">
-        <v>318</v>
-      </c>
-      <c r="C186" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D186" s="3">
-        <v>318</v>
-      </c>
-      <c r="E186" s="6">
-        <v>42990.77134259259</v>
-      </c>
-      <c r="F186" s="11" t="s">
-        <v>11</v>
+      <c r="D186" s="13">
+        <v>2576</v>
+      </c>
+      <c r="E186" s="14">
+        <v>43304.752638888887</v>
+      </c>
+      <c r="F186" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A187" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B187" s="3">
-        <v>1009</v>
+        <v>1237</v>
       </c>
       <c r="C187" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D187" s="3">
-        <v>1009</v>
+        <v>1237</v>
       </c>
       <c r="E187" s="6">
-        <v>44852.670138888891</v>
+        <v>43710.58252314815</v>
       </c>
       <c r="F187" s="11" t="s">
         <v>11</v>
@@ -6404,19 +6398,19 @@
     </row>
     <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A188" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B188" s="3">
-        <v>1657</v>
+        <v>872</v>
       </c>
       <c r="C188" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D188" s="3">
-        <v>1657</v>
+        <v>872</v>
       </c>
       <c r="E188" s="6">
-        <v>42990.765023148146</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F188" s="11" t="s">
         <v>11</v>
@@ -6424,372 +6418,372 @@
     </row>
     <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A189" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B189" s="3">
-        <v>1677</v>
+        <v>2471</v>
       </c>
       <c r="C189" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322094907409</v>
       </c>
       <c r="D189" s="3">
-        <v>1677</v>
+        <v>2471</v>
       </c>
       <c r="E189" s="6">
-        <v>44848.55972222222</v>
+        <v>42949.567870370367</v>
       </c>
       <c r="F189" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A190" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B190" s="13">
-        <v>2576</v>
-      </c>
-      <c r="C190" s="14">
+    <row r="190" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A190" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B190" s="3"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="3"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="11"/>
+    </row>
+    <row r="191" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A191" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B191" s="13">
+        <v>492</v>
+      </c>
+      <c r="C191" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D190" s="13">
-        <v>2576</v>
-      </c>
-      <c r="E190" s="14">
-        <v>43304.752638888887</v>
-      </c>
-      <c r="F190" s="13" t="s">
+      <c r="D191" s="13">
+        <v>492</v>
+      </c>
+      <c r="E191" s="14">
+        <v>44868.679872685185</v>
+      </c>
+      <c r="F191" s="13" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A191" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B191" s="3">
-        <v>1237</v>
-      </c>
-      <c r="C191" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D191" s="3">
-        <v>1237</v>
-      </c>
-      <c r="E191" s="6">
-        <v>43710.58252314815</v>
-      </c>
-      <c r="F191" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A192" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B192" s="3">
-        <v>872</v>
+        <v>1135</v>
       </c>
       <c r="C192" s="6">
-        <v>45533.322094907409</v>
+        <v>45637.672824074078</v>
       </c>
       <c r="D192" s="3">
-        <v>872</v>
+        <v>1267</v>
       </c>
       <c r="E192" s="6">
-        <v>42949.567847222221</v>
+        <v>44869.576215277775</v>
       </c>
       <c r="F192" s="11" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A193" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B193" s="3">
-        <v>2471</v>
+        <v>3316</v>
       </c>
       <c r="C193" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D193" s="3">
-        <v>2471</v>
+        <v>3316</v>
       </c>
       <c r="E193" s="6">
-        <v>42949.567870370367</v>
+        <v>44869.449074074073</v>
       </c>
       <c r="F193" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A194" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B194" s="3"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="3"/>
-      <c r="E194" s="6"/>
-      <c r="F194" s="11"/>
-    </row>
-    <row r="195" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B195" s="13">
-        <v>492</v>
-      </c>
-      <c r="C195" s="14">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D195" s="13">
-        <v>492</v>
-      </c>
-      <c r="E195" s="14">
-        <v>44868.679872685185</v>
-      </c>
-      <c r="F195" s="13" t="s">
-        <v>110</v>
+    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A194" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B194" s="3">
+        <v>2293</v>
+      </c>
+      <c r="C194" s="6">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D194" s="3">
+        <v>2293</v>
+      </c>
+      <c r="E194" s="6">
+        <v>44869.446643518517</v>
+      </c>
+      <c r="F194" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A195" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B195" s="3">
+        <v>2288</v>
+      </c>
+      <c r="C195" s="6">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D195" s="3">
+        <v>2288</v>
+      </c>
+      <c r="E195" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F195" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A196" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B196" s="3">
-        <v>1135</v>
+        <v>364</v>
       </c>
       <c r="C196" s="6">
-        <v>45637.672824074078</v>
+        <v>45533.322106481479</v>
       </c>
       <c r="D196" s="3">
-        <v>1267</v>
+        <v>364</v>
       </c>
       <c r="E196" s="6">
-        <v>44869.576215277775</v>
+        <v>43863.785486111112</v>
       </c>
       <c r="F196" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A197" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B197" s="3"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="11"/>
+    </row>
+    <row r="198" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A198" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B198" s="22">
+        <v>4763</v>
+      </c>
+      <c r="C198" s="23">
+        <v>45622.614722222221</v>
+      </c>
+      <c r="D198" s="22">
+        <v>4832</v>
+      </c>
+      <c r="E198" s="23">
+        <v>44869.413148148145</v>
+      </c>
+      <c r="F198" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H198" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A199" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B199" s="13">
+        <v>483</v>
+      </c>
+      <c r="C199" s="14">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D199" s="13">
+        <v>483</v>
+      </c>
+      <c r="E199" s="14">
+        <v>42992.768796296295</v>
+      </c>
+      <c r="F199" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A200" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B200" s="13">
+        <v>743</v>
+      </c>
+      <c r="C200" s="14">
+        <v>45637.479016203702</v>
+      </c>
+      <c r="D200" s="13">
+        <v>836</v>
+      </c>
+      <c r="E200" s="14">
+        <v>44869.403402777774</v>
+      </c>
+      <c r="F200" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A201" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B201" s="13">
+        <v>749</v>
+      </c>
+      <c r="C201" s="14">
+        <v>45637.479409722226</v>
+      </c>
+      <c r="D201" s="13">
+        <v>761</v>
+      </c>
+      <c r="E201" s="14">
+        <v>44869.396956018521</v>
+      </c>
+      <c r="F201" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A202" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" s="13">
+        <v>451</v>
+      </c>
+      <c r="C202" s="14">
+        <v>45637.539085648146</v>
+      </c>
+      <c r="D202" s="13">
+        <v>401</v>
+      </c>
+      <c r="E202" s="14">
+        <v>42999.700740740744</v>
+      </c>
+      <c r="F202" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A203" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B203" s="3"/>
+      <c r="C203" s="6"/>
+      <c r="D203" s="3"/>
+      <c r="E203" s="6"/>
+      <c r="F203" s="11"/>
+    </row>
+    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A204" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B204" s="3">
+        <v>815</v>
+      </c>
+      <c r="C204" s="6">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D204" s="3">
+        <v>815</v>
+      </c>
+      <c r="E204" s="6">
+        <v>44865.586435185185</v>
+      </c>
+      <c r="F204" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A205" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B205" s="3">
+        <v>2674</v>
+      </c>
+      <c r="C205" s="6">
+        <v>45637.463252314818</v>
+      </c>
+      <c r="D205" s="3">
+        <v>2649</v>
+      </c>
+      <c r="E205" s="6">
+        <v>44869.507557870369</v>
+      </c>
+      <c r="F205" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A197" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B197" s="3">
-        <v>3316</v>
-      </c>
-      <c r="C197" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D197" s="3">
-        <v>3316</v>
-      </c>
-      <c r="E197" s="6">
-        <v>44869.449074074073</v>
-      </c>
-      <c r="F197" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A198" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B198" s="3">
-        <v>2293</v>
-      </c>
-      <c r="C198" s="6">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D198" s="3">
-        <v>2293</v>
-      </c>
-      <c r="E198" s="6">
-        <v>44869.446643518517</v>
-      </c>
-      <c r="F198" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A199" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B199" s="3">
-        <v>2288</v>
-      </c>
-      <c r="C199" s="6">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D199" s="3">
-        <v>2288</v>
-      </c>
-      <c r="E199" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F199" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A200" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B200" s="3">
-        <v>364</v>
-      </c>
-      <c r="C200" s="6">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D200" s="3">
-        <v>364</v>
-      </c>
-      <c r="E200" s="6">
-        <v>43863.785486111112</v>
-      </c>
-      <c r="F200" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A201" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B201" s="3"/>
-      <c r="C201" s="6"/>
-      <c r="D201" s="3"/>
-      <c r="E201" s="6"/>
-      <c r="F201" s="11"/>
-    </row>
-    <row r="202" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A202" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="B202" s="22">
-        <v>4763</v>
-      </c>
-      <c r="C202" s="23">
-        <v>45622.614722222221</v>
-      </c>
-      <c r="D202" s="22">
-        <v>4832</v>
-      </c>
-      <c r="E202" s="23">
-        <v>44869.413148148145</v>
-      </c>
-      <c r="F202" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H202" s="22" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A203" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B203" s="13">
-        <v>483</v>
-      </c>
-      <c r="C203" s="14">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D203" s="13">
-        <v>483</v>
-      </c>
-      <c r="E203" s="14">
-        <v>42992.768796296295</v>
-      </c>
-      <c r="F203" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A204" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B204" s="13">
-        <v>743</v>
-      </c>
-      <c r="C204" s="14">
-        <v>45637.479016203702</v>
-      </c>
-      <c r="D204" s="13">
-        <v>836</v>
-      </c>
-      <c r="E204" s="14">
-        <v>44869.403402777774</v>
-      </c>
-      <c r="F204" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A205" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B205" s="13">
-        <v>749</v>
-      </c>
-      <c r="C205" s="14">
-        <v>45637.479409722226</v>
-      </c>
-      <c r="D205" s="13">
-        <v>761</v>
-      </c>
-      <c r="E205" s="14">
-        <v>44869.396956018521</v>
-      </c>
-      <c r="F205" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A206" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B206" s="13">
-        <v>451</v>
-      </c>
-      <c r="C206" s="14">
-        <v>45637.539085648146</v>
-      </c>
-      <c r="D206" s="13">
-        <v>401</v>
-      </c>
-      <c r="E206" s="14">
-        <v>42999.700740740744</v>
-      </c>
-      <c r="F206" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A207" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="B207" s="3"/>
-      <c r="C207" s="6"/>
-      <c r="D207" s="3"/>
-      <c r="E207" s="6"/>
-      <c r="F207" s="11"/>
+    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A206" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B206" s="3">
+        <v>162</v>
+      </c>
+      <c r="C206" s="6">
+        <v>45533.322118055556</v>
+      </c>
+      <c r="D206" s="3">
+        <v>162</v>
+      </c>
+      <c r="E206" s="6">
+        <v>42949.567870370367</v>
+      </c>
+      <c r="F206" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A207" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B207" s="3">
+        <v>286</v>
+      </c>
+      <c r="C207" s="6">
+        <v>45533.322118055556</v>
+      </c>
+      <c r="D207" s="3">
+        <v>286</v>
+      </c>
+      <c r="E207" s="6">
+        <v>44861.727037037039</v>
+      </c>
+      <c r="F207" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A208" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B208" s="3">
-        <v>815</v>
+        <v>255</v>
       </c>
       <c r="C208" s="6">
-        <v>45533.322106481479</v>
+        <v>45533.322118055556</v>
       </c>
       <c r="D208" s="3">
-        <v>815</v>
+        <v>255</v>
       </c>
       <c r="E208" s="6">
-        <v>44865.586435185185</v>
+        <v>44861.727152777778</v>
       </c>
       <c r="F208" s="11" t="s">
         <v>11</v>
@@ -6797,146 +6791,80 @@
     </row>
     <row r="209" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A209" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B209" s="3">
-        <v>2674</v>
+        <v>420</v>
       </c>
       <c r="C209" s="6">
-        <v>45637.463252314818</v>
+        <v>45533.322118055556</v>
       </c>
       <c r="D209" s="3">
-        <v>2649</v>
+        <v>420</v>
       </c>
       <c r="E209" s="6">
-        <v>44869.507557870369</v>
+        <v>44861.727546296293</v>
       </c>
       <c r="F209" s="11" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A210" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B210" s="3">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C210" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D210" s="3">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E210" s="6">
-        <v>42949.567870370367</v>
+        <v>44869.508900462963</v>
       </c>
       <c r="F210" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A211" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B211" s="3">
-        <v>286</v>
-      </c>
-      <c r="C211" s="6">
-        <v>45533.322118055556</v>
-      </c>
-      <c r="D211" s="3">
-        <v>286</v>
-      </c>
-      <c r="E211" s="6">
-        <v>44861.727037037039</v>
-      </c>
-      <c r="F211" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A212" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B212" s="3">
-        <v>255</v>
-      </c>
-      <c r="C212" s="6">
-        <v>45533.322118055556</v>
-      </c>
-      <c r="D212" s="3">
-        <v>255</v>
-      </c>
-      <c r="E212" s="6">
-        <v>44861.727152777778</v>
-      </c>
-      <c r="F212" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A213" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B213" s="3">
-        <v>420</v>
-      </c>
-      <c r="C213" s="6">
-        <v>45533.322118055556</v>
-      </c>
-      <c r="D213" s="3">
-        <v>420</v>
-      </c>
-      <c r="E213" s="6">
-        <v>44861.727546296293</v>
-      </c>
-      <c r="F213" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A214" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B214" s="3">
-        <v>138</v>
-      </c>
-      <c r="C214" s="6">
-        <v>45533.322118055556</v>
-      </c>
-      <c r="D214" s="3">
-        <v>138</v>
-      </c>
-      <c r="E214" s="6">
-        <v>44869.508900462963</v>
-      </c>
-      <c r="F214" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A215" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="B215" s="22">
+    <row r="211" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A211" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B211" s="22">
         <v>11219</v>
       </c>
-      <c r="C215" s="23">
+      <c r="C211" s="23">
         <v>45636.606886574074</v>
       </c>
-      <c r="D215" s="22">
+      <c r="D211" s="22">
         <v>13055</v>
       </c>
-      <c r="E215" s="23">
+      <c r="E211" s="23">
         <v>44869.593541666669</v>
       </c>
-      <c r="F215" s="22" t="s">
+      <c r="F211" s="22" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B7:C7"/>
@@ -6949,27 +6877,13 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B81:C81"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D108 A109:B110 D109:E110 A111:E111 A112:B116 D112:E116 A117:E123 A124:D124 B125:D127 A128:D128 A129:E150 B151:E151 A152:E215">
+  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D104 A105:B106 D105:E106 A107:E107 A108:B112 D108:E112 A113:E119 A120:D120 B121:D123 A124:D124 A125:E146 B147:E147 A148:E211">
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="/.">
       <formula>NOT(ISERROR(SEARCH("/.",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 A77:E124 G77:XFD162 B125:E127 A128:E150 B151:E151 A152:E215 G163 I163:XFD163 G164:XFD215 A216:XFD1048576">
+  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 B121:E123 A124:E146 B147:E147 A148:E211 G159 I159:XFD159 G160:XFD211 A212:XFD1048576 A77:E120 G77:XFD158">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
@@ -6994,10 +6908,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="31" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to TTL triggering
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukhina\Documents\MATLAB\ScopeScript-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CAA528-567E-40E7-A907-0FD40E1A8239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFA29FB-E195-4CD0-8617-F01EE36F9920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{64517161-2A91-2B47-8856-8DF463AC8E32}"/>
   </bookViews>
@@ -17,9 +17,9 @@
     <sheet name="Arduino code check list" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Matlab Code Check List'!$A$1:$F$212</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="249">
   <si>
     <r>
       <t>Left file list</t>
@@ -879,202 +879,7 @@
   </si>
   <si>
     <r>
-      <t>imagingControl/executeFunctionsControl/executeFunctions.m  (open: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>left</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t> | </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>imagingControl/executeFunctionsControl/executeFunctionsInFcScopeList.m  (open: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>left</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t> | </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>imagingControl/executeFunctionsControl/initForNextInFcScopeList.m  (open: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>left</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t> | </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>imagingControl/executeFunctionsControl/parseParamsForFunctions.m  (open: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>left</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t> | </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>imagingControl/executeFunctionsControl/updateChannelGivenCommand.m  (open: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>left</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t> | </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>imagingControl/timeLapseControl/doTimeLapse.m  (open: </t>
     </r>
     <r>
       <rPr>
@@ -1498,9 +1303,6 @@
     <t>hardwareControl/light_sources/mapChannelToFilterCube.m  (open)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +/- need to add filtercube for UV LED once it arrives</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +/- re-check later; OK for now; need to add default TIRF settings</t>
   </si>
   <si>
@@ -1924,9 +1726,6 @@
   </si>
   <si>
     <t>dataManagement/returnDate.m  (open: left | right)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +/- check with TTL triggering - what mmc.setProperty('UV LED','UV340') does?</t>
   </si>
   <si>
     <t>hardwareControl/light_sources/laser/turnOnAllLasers.m  (open: left | right)</t>
@@ -2101,9 +1900,6 @@
     <t>hardwareControl/piezoController/holdPiezoBF.m  (open: left | right)</t>
   </si>
   <si>
-    <t>commented ttlPiezo(); check what is done by shapeInserter = vision.ShapeInserter</t>
-  </si>
-  <si>
     <t>imagingControl/live/doLive.m  (open: left | right)</t>
   </si>
   <si>
@@ -2202,12 +1998,6 @@
     <t>constantPiezoLightsOn.m</t>
   </si>
   <si>
-    <t>"Fast USB to Serial" --&gt; enabled for COM7 (Toptica) and COM4 (Arduino)</t>
-  </si>
-  <si>
-    <t>!!!!CHECK FOR STABILITY - supposed to speed up communication by 10x</t>
-  </si>
-  <si>
     <t>mapChannelToMirrorPosition</t>
   </si>
   <si>
@@ -2223,7 +2013,40 @@
     <t>hardwareControl/light_sources/BF_LED/turnONBFLED.m  (open)</t>
   </si>
   <si>
-    <t>redundant? Check for dependencies other than in setupChannel</t>
+    <t>commented parpool for now; uncomment when everything is done</t>
+  </si>
+  <si>
+    <t>printCurrentBFLightSourceState</t>
+  </si>
+  <si>
+    <t>"Fast USB to Serial" --&gt; enabled for COM7 (Toptica) and disabled for COM4 (Arduino)</t>
+  </si>
+  <si>
+    <t>!!!!CHECK FOR STABILITY - supposed to speed up communication by 10x; try to enable for arduino later</t>
+  </si>
+  <si>
+    <t>commented ttlPiezo() - seems to be fine; tested e,p,s,q with BF and PL; check what is done by shapeInserter = vision.ShapeInserter</t>
+  </si>
+  <si>
+    <t>imagingControl/executeFunctionsControl/executeFunctions.m  (open: left | right)</t>
+  </si>
+  <si>
+    <t>imagingControl/executeFunctionsControl/executeFunctionsInFcScopeList.m  (open: left | right)</t>
+  </si>
+  <si>
+    <t>tested with simple channel recipies for BF and laser; needs more tests once the channel recipies are finalized</t>
+  </si>
+  <si>
+    <t>imagingControl/executeFunctionsControl/updateChannelGivenCommand.m  (open: left | right)</t>
+  </si>
+  <si>
+    <t>imagingControl/executeFunctionsControl/parseParamsForFunctions.m  (open: left | right)</t>
+  </si>
+  <si>
+    <t>imagingControl/timeLapseControl/doTimeLapse.m  (open: left | right)</t>
+  </si>
+  <si>
+    <t>need to test</t>
   </si>
 </sst>
 </file>
@@ -2535,16 +2358,16 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2553,7 +2376,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2912,11 +2755,11 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <pane ySplit="8" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2932,7 +2775,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.4">
@@ -2940,7 +2783,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.4">
@@ -2957,14 +2800,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="34"/>
+      <c r="B7" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
@@ -2986,12 +2829,12 @@
         <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3002,12 +2845,12 @@
     </row>
     <row r="10" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="22">
         <v>835</v>
       </c>
@@ -3018,17 +2861,17 @@
         <v>10</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="B11" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="22">
         <v>2953</v>
       </c>
@@ -3039,17 +2882,17 @@
         <v>10</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="B12" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="22">
         <v>406</v>
       </c>
@@ -3060,17 +2903,17 @@
         <v>10</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B13" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="22">
         <v>5488</v>
       </c>
@@ -3081,17 +2924,17 @@
         <v>10</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="22">
         <v>634</v>
       </c>
@@ -3102,17 +2945,17 @@
         <v>10</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="B15" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="22">
         <v>510</v>
       </c>
@@ -3123,17 +2966,17 @@
         <v>10</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="22">
         <v>771</v>
       </c>
@@ -3144,17 +2987,17 @@
         <v>10</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="22">
         <v>1203</v>
       </c>
@@ -3165,17 +3008,17 @@
         <v>10</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="22">
         <v>594</v>
       </c>
@@ -3186,17 +3029,17 @@
         <v>10</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B19" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="22">
         <v>962</v>
       </c>
@@ -3207,17 +3050,17 @@
         <v>10</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="B20" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="22">
         <v>1255</v>
       </c>
@@ -3228,17 +3071,17 @@
         <v>10</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="22">
         <v>2288</v>
       </c>
@@ -3249,17 +3092,17 @@
         <v>10</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="22">
         <v>1552</v>
       </c>
@@ -3270,17 +3113,17 @@
         <v>10</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="B23" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="22">
         <v>764</v>
       </c>
@@ -3291,17 +3134,17 @@
         <v>10</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="B24" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="22">
         <v>342</v>
       </c>
@@ -3312,12 +3155,12 @@
         <v>10</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" s="24" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3328,7 +3171,7 @@
     </row>
     <row r="26" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B26" s="13">
         <v>323</v>
@@ -3343,15 +3186,15 @@
         <v>44846.595555555556</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B27" s="22">
         <v>1555</v>
@@ -3369,12 +3212,12 @@
         <v>11</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B28" s="22">
         <v>1477</v>
@@ -3392,12 +3235,12 @@
         <v>11</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B29" s="22">
         <v>197</v>
@@ -3415,12 +3258,12 @@
         <v>11</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B30" s="22">
         <v>1111</v>
@@ -3438,12 +3281,12 @@
         <v>11</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B31" s="22">
         <v>1235</v>
@@ -3461,12 +3304,12 @@
         <v>11</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B32" s="22">
         <v>755</v>
@@ -3484,12 +3327,12 @@
         <v>11</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B33" s="22">
         <v>342</v>
@@ -3507,12 +3350,12 @@
         <v>11</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B34" s="22">
         <v>169</v>
@@ -3530,12 +3373,12 @@
         <v>11</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B35" s="22">
         <v>237</v>
@@ -3553,12 +3396,12 @@
         <v>11</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B36" s="22">
         <v>432</v>
@@ -3576,12 +3419,12 @@
         <v>11</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B37" s="22">
         <v>3069</v>
@@ -3599,12 +3442,12 @@
         <v>11</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B38" s="22">
         <v>303</v>
@@ -3622,12 +3465,12 @@
         <v>11</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B39" s="22">
         <v>698</v>
@@ -3645,12 +3488,12 @@
         <v>11</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B40" s="22">
         <v>605</v>
@@ -3668,12 +3511,12 @@
         <v>11</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B41" s="22">
         <v>988</v>
@@ -3691,12 +3534,12 @@
         <v>11</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="22" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B42" s="22">
         <v>387</v>
@@ -3714,12 +3557,12 @@
         <v>11</v>
       </c>
       <c r="H42" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="22" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B43" s="22">
         <v>5585</v>
@@ -3737,12 +3580,12 @@
         <v>11</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B44" s="22">
         <v>2983</v>
@@ -3757,15 +3600,15 @@
         <v>44865.695856481485</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B45" s="22">
         <v>1103</v>
@@ -3783,12 +3626,12 @@
         <v>11</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B46" s="22">
         <v>381</v>
@@ -3806,12 +3649,12 @@
         <v>11</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B47" s="22">
         <v>674</v>
@@ -3829,12 +3672,12 @@
         <v>11</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="22" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B48" s="22">
         <v>1481</v>
@@ -3852,12 +3695,12 @@
         <v>11</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="22" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B49" s="22">
         <v>1078</v>
@@ -3875,12 +3718,12 @@
         <v>11</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="22" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B50" s="22">
         <v>833</v>
@@ -3898,12 +3741,12 @@
         <v>11</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="22" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B51" s="22">
         <v>817</v>
@@ -3921,12 +3764,12 @@
         <v>11</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B52" s="22">
         <v>188</v>
@@ -3944,12 +3787,12 @@
         <v>11</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="22" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B53" s="22">
         <v>221</v>
@@ -3967,12 +3810,12 @@
         <v>11</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="20" x14ac:dyDescent="0.4">
       <c r="A54" s="26" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="6"/>
@@ -3983,7 +3826,7 @@
     </row>
     <row r="55" spans="1:8" ht="20" x14ac:dyDescent="0.4">
       <c r="A55" s="26" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="6"/>
@@ -3994,7 +3837,7 @@
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B56" s="22">
         <v>1217</v>
@@ -4012,12 +3855,12 @@
         <v>11</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B57" s="13">
         <v>611</v>
@@ -4032,12 +3875,12 @@
         <v>44862.461018518516</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B58" s="13">
         <v>617</v>
@@ -4052,12 +3895,12 @@
         <v>44862.46266203704</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B59" s="15">
         <v>159</v>
@@ -4077,7 +3920,7 @@
     </row>
     <row r="60" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B60" s="15">
         <v>145</v>
@@ -4097,7 +3940,7 @@
     </row>
     <row r="61" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B61" s="15">
         <v>145</v>
@@ -4117,7 +3960,7 @@
     </row>
     <row r="62" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B62" s="15">
         <v>176</v>
@@ -4137,7 +3980,7 @@
     </row>
     <row r="63" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B63" s="15">
         <v>283</v>
@@ -4157,7 +4000,7 @@
     </row>
     <row r="64" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B64" s="13">
         <v>209</v>
@@ -4172,15 +4015,15 @@
         <v>43398.915833333333</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B65" s="15">
         <v>171</v>
@@ -4200,7 +4043,7 @@
     </row>
     <row r="66" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B66" s="15">
         <v>376</v>
@@ -4220,12 +4063,12 @@
     </row>
     <row r="67" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A67" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="36"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="17">
         <v>314</v>
       </c>
@@ -4238,12 +4081,12 @@
     </row>
     <row r="68" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A68" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="36"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="17">
         <v>308</v>
       </c>
@@ -4256,7 +4099,7 @@
     </row>
     <row r="69" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B69" s="15">
         <v>828</v>
@@ -4276,7 +4119,7 @@
     </row>
     <row r="70" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B70" s="13">
         <v>130</v>
@@ -4291,12 +4134,12 @@
         <v>44865.503148148149</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B71" s="15">
         <v>148</v>
@@ -4316,7 +4159,7 @@
     </row>
     <row r="72" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B72" s="15">
         <v>198</v>
@@ -4336,7 +4179,7 @@
     </row>
     <row r="73" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B73" s="15">
         <v>131</v>
@@ -4356,17 +4199,17 @@
     </row>
     <row r="74" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A74" s="25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A75" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B75" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="36"/>
+      <c r="C75" s="34"/>
       <c r="D75" s="17">
         <v>286</v>
       </c>
@@ -4379,7 +4222,7 @@
     </row>
     <row r="76" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B76" s="13">
         <v>1103</v>
@@ -4397,17 +4240,17 @@
         <v>11</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A77" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B77" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="38"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="7">
         <v>833</v>
       </c>
@@ -4420,7 +4263,7 @@
     </row>
     <row r="78" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B78" s="13">
         <v>564</v>
@@ -4435,12 +4278,12 @@
         <v>9</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B79" s="15">
         <v>966</v>
@@ -4455,40 +4298,37 @@
         <v>44865.62122685185</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B80" s="13">
         <v>89</v>
       </c>
-      <c r="C80" s="16">
+      <c r="C80" s="14">
         <v>45637.519189814811</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="15" t="s">
+      <c r="F80" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="H80" s="15" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B81" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="38"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="7">
         <v>2626</v>
       </c>
@@ -4501,7 +4341,7 @@
     </row>
     <row r="82" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B82" s="13">
         <v>365</v>
@@ -4521,7 +4361,7 @@
     </row>
     <row r="83" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B83" s="13">
         <v>702</v>
@@ -4536,12 +4376,12 @@
         <v>44862.410416666666</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B84" s="13">
         <v>344</v>
@@ -4556,60 +4396,57 @@
         <v>44866.7030787037</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B85" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" s="15">
         <v>964</v>
       </c>
-      <c r="C85" s="14">
+      <c r="C85" s="16">
         <v>45639.658865740741</v>
       </c>
-      <c r="D85" s="13">
+      <c r="D85" s="15">
         <v>808</v>
       </c>
-      <c r="E85" s="14">
+      <c r="E85" s="16">
         <v>44865.582754629628</v>
       </c>
-      <c r="F85" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H85" s="13" t="s">
-        <v>88</v>
+      <c r="F85" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A86" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B87" s="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B87" s="13">
         <v>375</v>
       </c>
-      <c r="C87" s="16">
+      <c r="C87" s="14">
         <v>45636.639525462961</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F87" s="15" t="s">
+      <c r="F87" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="H87" s="15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B88" s="13">
         <v>304</v>
@@ -4626,7 +4463,7 @@
     </row>
     <row r="89" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B89" s="13">
         <v>3565</v>
@@ -4643,7 +4480,7 @@
     </row>
     <row r="90" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B90" s="13">
         <v>102</v>
@@ -4658,15 +4495,15 @@
         <v>42991.860717592594</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="20" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B91" s="20">
         <v>159</v>
@@ -4684,12 +4521,12 @@
         <v>10</v>
       </c>
       <c r="H91" s="20" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C92" s="14"/>
       <c r="E92" s="14"/>
@@ -4699,7 +4536,7 @@
     </row>
     <row r="93" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A93" s="28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="6"/>
@@ -4708,12 +4545,12 @@
     </row>
     <row r="94" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A94" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B94" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="37"/>
+      <c r="C94" s="35"/>
       <c r="D94" s="17">
         <v>709</v>
       </c>
@@ -4726,7 +4563,7 @@
     </row>
     <row r="95" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B95" s="20">
         <v>155</v>
@@ -4746,7 +4583,7 @@
     </row>
     <row r="96" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="20" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B96" s="20">
         <v>1545</v>
@@ -4766,7 +4603,7 @@
     </row>
     <row r="97" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="20" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B97" s="20">
         <v>136</v>
@@ -4786,7 +4623,7 @@
     </row>
     <row r="98" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="20" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B98" s="20">
         <v>109</v>
@@ -4804,12 +4641,12 @@
         <v>10</v>
       </c>
       <c r="H98" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A99" s="15" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C99" s="16"/>
       <c r="E99" s="16"/>
@@ -4817,12 +4654,12 @@
         <v>9</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" s="15" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C100" s="16"/>
       <c r="E100" s="16"/>
@@ -4830,12 +4667,12 @@
         <v>9</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C101" s="16"/>
       <c r="E101" s="16"/>
@@ -4843,12 +4680,12 @@
         <v>9</v>
       </c>
       <c r="H101" s="15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A102" s="28" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="6"/>
@@ -4858,7 +4695,7 @@
     </row>
     <row r="103" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A103" s="13" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B103" s="13">
         <v>196</v>
@@ -4875,7 +4712,7 @@
     </row>
     <row r="104" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A104" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B104" s="15">
         <v>394</v>
@@ -4890,174 +4727,165 @@
         <v>9</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A105" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B105" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="F105" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A106" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D105" s="17">
+      <c r="D106" s="17">
         <v>262</v>
       </c>
-      <c r="E105" s="18">
+      <c r="E106" s="18">
         <v>42962.894861111112</v>
       </c>
-      <c r="F105" s="19" t="s">
+      <c r="F106" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B106" s="20" t="s">
+    <row r="107" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D106" s="20">
+      <c r="D107" s="20">
         <v>464</v>
       </c>
-      <c r="E106" s="20">
+      <c r="E107" s="20">
         <v>44862.503541666665</v>
       </c>
-      <c r="F106" s="20" t="s">
+      <c r="F107" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A107" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B107" s="17">
+    <row r="108" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A108" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B108" s="17">
         <v>4585</v>
       </c>
-      <c r="C107" s="18">
+      <c r="C108" s="18">
         <v>45533.321979166663</v>
       </c>
-      <c r="D107" s="17">
+      <c r="D108" s="17">
         <v>4585</v>
       </c>
-      <c r="E107" s="18">
+      <c r="E108" s="18">
         <v>44390.836111111108</v>
       </c>
-      <c r="F107" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B108" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C108" s="35"/>
-      <c r="D108" s="20">
-        <v>1225</v>
-      </c>
-      <c r="E108" s="20">
-        <v>44862.499490740738</v>
-      </c>
-      <c r="F108" s="20" t="s">
+      <c r="F108" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B109" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B109" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C109" s="35"/>
+      <c r="C109" s="33"/>
       <c r="D109" s="20">
-        <v>1053</v>
+        <v>1225</v>
       </c>
       <c r="E109" s="20">
-        <v>44862.498703703706</v>
+        <v>44862.499490740738</v>
       </c>
       <c r="F109" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A110" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B110" s="36" t="s">
+    <row r="110" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B110" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C110" s="36"/>
-      <c r="D110" s="17">
+      <c r="C110" s="33"/>
+      <c r="D110" s="20">
+        <v>1053</v>
+      </c>
+      <c r="E110" s="20">
+        <v>44862.498703703706</v>
+      </c>
+      <c r="F110" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A111" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="34"/>
+      <c r="D111" s="17">
         <v>6709</v>
       </c>
-      <c r="E110" s="18">
+      <c r="E111" s="18">
         <v>44868.709155092591</v>
       </c>
-      <c r="F110" s="19" t="s">
+      <c r="F111" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B111" s="20" t="s">
+    <row r="112" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D111" s="20">
+      <c r="D112" s="20">
         <v>285</v>
       </c>
-      <c r="E111" s="20">
+      <c r="E112" s="20">
         <v>44846.595578703702</v>
       </c>
-      <c r="F111" s="20" t="s">
+      <c r="F112" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A112" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A113" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B113" s="13">
-        <v>316</v>
-      </c>
-      <c r="C113" s="14">
-        <v>45533.322002314817</v>
-      </c>
-      <c r="D113" s="13">
-        <v>316</v>
-      </c>
-      <c r="E113" s="14">
-        <v>42977.691412037035</v>
-      </c>
-      <c r="F113" s="13" t="s">
-        <v>11</v>
+    <row r="113" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+      <c r="A113" s="27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A114" s="13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B114" s="13">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="C114" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D114" s="13">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="E114" s="14">
-        <v>44852.729004629633</v>
+        <v>42977.691412037035</v>
       </c>
       <c r="F114" s="13" t="s">
         <v>11</v>
@@ -5065,19 +4893,19 @@
     </row>
     <row r="115" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A115" s="13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B115" s="13">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="C115" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D115" s="13">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E115" s="14">
-        <v>44852.731087962966</v>
+        <v>44852.729004629633</v>
       </c>
       <c r="F115" s="13" t="s">
         <v>11</v>
@@ -5085,19 +4913,19 @@
     </row>
     <row r="116" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A116" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B116" s="13">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="C116" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D116" s="13">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="E116" s="14">
-        <v>44865.57439814815</v>
+        <v>44852.731087962966</v>
       </c>
       <c r="F116" s="13" t="s">
         <v>11</v>
@@ -5105,19 +4933,19 @@
     </row>
     <row r="117" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B117" s="13">
-        <v>304</v>
+        <v>223</v>
       </c>
       <c r="C117" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D117" s="13">
-        <v>304</v>
+        <v>223</v>
       </c>
       <c r="E117" s="14">
-        <v>44865.574004629627</v>
+        <v>44865.57439814815</v>
       </c>
       <c r="F117" s="13" t="s">
         <v>11</v>
@@ -5125,58 +4953,69 @@
     </row>
     <row r="118" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B118" s="13">
-        <v>1449</v>
+        <v>304</v>
       </c>
       <c r="C118" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D118" s="13">
+        <v>304</v>
+      </c>
+      <c r="E118" s="14">
+        <v>44865.574004629627</v>
+      </c>
+      <c r="F118" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B119" s="13">
         <v>1449</v>
       </c>
-      <c r="E118" s="14">
+      <c r="C119" s="14">
+        <v>45533.322002314817</v>
+      </c>
+      <c r="D119" s="13">
+        <v>1449</v>
+      </c>
+      <c r="E119" s="14">
         <v>44865.573680555557</v>
       </c>
-      <c r="F118" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="23.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A119" s="27" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A120" s="22" t="s">
+      <c r="F119" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="23.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A120" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A121" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B121" s="22">
         <v>199</v>
       </c>
-      <c r="B120" s="22">
-        <v>199</v>
-      </c>
-      <c r="C120" s="23">
+      <c r="C121" s="23">
         <v>45638.596597222226</v>
       </c>
-      <c r="D120" s="22" t="s">
+      <c r="D121" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F120" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A121" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="C121" s="14"/>
-      <c r="F121" s="13" t="s">
+      <c r="F121" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" s="29" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C122" s="14"/>
       <c r="F122" s="13" t="s">
@@ -5185,57 +5024,46 @@
     </row>
     <row r="123" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" s="29" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="C123" s="14"/>
       <c r="F123" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A124" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B124" s="3"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="5"/>
-      <c r="F124" s="11"/>
-    </row>
-    <row r="125" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A125" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B125" s="13">
-        <v>257</v>
-      </c>
-      <c r="C125" s="14">
-        <v>45533.322002314817</v>
-      </c>
-      <c r="D125" s="13">
-        <v>257</v>
-      </c>
-      <c r="E125" s="14">
-        <v>42978.469814814816</v>
-      </c>
-      <c r="F125" s="13" t="s">
-        <v>11</v>
-      </c>
+    <row r="124" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C124" s="14"/>
+      <c r="F124" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+      <c r="A125" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" s="3"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="5"/>
+      <c r="F125" s="11"/>
     </row>
     <row r="126" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="13" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B126" s="13">
-        <v>536</v>
+        <v>257</v>
       </c>
       <c r="C126" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D126" s="13">
-        <v>536</v>
+        <v>257</v>
       </c>
       <c r="E126" s="14">
-        <v>42978.465370370373</v>
+        <v>42978.469814814816</v>
       </c>
       <c r="F126" s="13" t="s">
         <v>11</v>
@@ -5243,19 +5071,19 @@
     </row>
     <row r="127" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B127" s="13">
-        <v>472</v>
+        <v>536</v>
       </c>
       <c r="C127" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D127" s="13">
-        <v>472</v>
+        <v>536</v>
       </c>
       <c r="E127" s="14">
-        <v>43041.741759259261</v>
+        <v>42978.465370370373</v>
       </c>
       <c r="F127" s="13" t="s">
         <v>11</v>
@@ -5263,19 +5091,19 @@
     </row>
     <row r="128" spans="1:6" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A128" s="13" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B128" s="13">
-        <v>257</v>
+        <v>472</v>
       </c>
       <c r="C128" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D128" s="13">
-        <v>257</v>
+        <v>472</v>
       </c>
       <c r="E128" s="14">
-        <v>42978.510162037041</v>
+        <v>43041.741759259261</v>
       </c>
       <c r="F128" s="13" t="s">
         <v>11</v>
@@ -5283,19 +5111,19 @@
     </row>
     <row r="129" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B129" s="13">
-        <v>741</v>
+        <v>257</v>
       </c>
       <c r="C129" s="14">
         <v>45533.322002314817</v>
       </c>
       <c r="D129" s="13">
-        <v>741</v>
+        <v>257</v>
       </c>
       <c r="E129" s="14">
-        <v>42978.451574074075</v>
+        <v>42978.510162037041</v>
       </c>
       <c r="F129" s="13" t="s">
         <v>11</v>
@@ -5303,19 +5131,19 @@
     </row>
     <row r="130" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B130" s="13">
-        <v>112</v>
+        <v>741</v>
       </c>
       <c r="C130" s="14">
-        <v>45533.322013888886</v>
+        <v>45533.322002314817</v>
       </c>
       <c r="D130" s="13">
-        <v>112</v>
+        <v>741</v>
       </c>
       <c r="E130" s="14">
-        <v>44865.577453703707</v>
+        <v>42978.451574074075</v>
       </c>
       <c r="F130" s="13" t="s">
         <v>11</v>
@@ -5323,19 +5151,19 @@
     </row>
     <row r="131" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B131" s="13">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="C131" s="14">
         <v>45533.322013888886</v>
       </c>
       <c r="D131" s="13">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E131" s="14">
-        <v>42977.54828703704</v>
+        <v>44865.577453703707</v>
       </c>
       <c r="F131" s="13" t="s">
         <v>11</v>
@@ -5343,19 +5171,19 @@
     </row>
     <row r="132" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B132" s="13">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="C132" s="14">
         <v>45533.322013888886</v>
       </c>
       <c r="D132" s="13">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="E132" s="14">
-        <v>42992.41233796296</v>
+        <v>42977.54828703704</v>
       </c>
       <c r="F132" s="13" t="s">
         <v>11</v>
@@ -5363,445 +5191,445 @@
     </row>
     <row r="133" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B133" s="13">
-        <v>310</v>
+        <v>125</v>
       </c>
       <c r="C133" s="14">
         <v>45533.322013888886</v>
       </c>
       <c r="D133" s="13">
+        <v>125</v>
+      </c>
+      <c r="E133" s="14">
+        <v>42992.41233796296</v>
+      </c>
+      <c r="F133" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B134" s="13">
         <v>310</v>
       </c>
-      <c r="E133" s="14">
+      <c r="C134" s="14">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D134" s="13">
+        <v>310</v>
+      </c>
+      <c r="E134" s="14">
         <v>44865.57775462963</v>
       </c>
-      <c r="F133" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A134" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B134" s="15">
-        <v>386</v>
-      </c>
-      <c r="C134" s="16">
-        <v>45533.322013888886</v>
-      </c>
-      <c r="D134" s="15">
-        <v>386</v>
-      </c>
-      <c r="E134" s="16">
-        <v>44865.615277777775</v>
-      </c>
-      <c r="F134" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H134" s="15" t="s">
-        <v>218</v>
+      <c r="F134" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B135" s="15">
-        <v>264</v>
+        <v>386</v>
       </c>
       <c r="C135" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D135" s="15">
-        <v>264</v>
+        <v>386</v>
       </c>
       <c r="E135" s="16">
-        <v>42989.788611111115</v>
+        <v>44865.615277777775</v>
       </c>
       <c r="F135" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H135" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A136" s="15" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B136" s="15">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="C136" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D136" s="15">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="E136" s="16">
-        <v>44865.616296296299</v>
+        <v>42989.788611111115</v>
       </c>
       <c r="F136" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H136" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" s="15" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B137" s="15">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="C137" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D137" s="15">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="E137" s="16">
-        <v>42989.793263888889</v>
+        <v>44865.616296296299</v>
       </c>
       <c r="F137" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H137" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B138" s="15">
-        <v>1048</v>
+        <v>284</v>
       </c>
       <c r="C138" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D138" s="15">
-        <v>1048</v>
+        <v>284</v>
       </c>
       <c r="E138" s="16">
-        <v>44869.567465277774</v>
+        <v>42989.793263888889</v>
       </c>
       <c r="F138" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H138" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B139" s="15">
-        <v>130</v>
+        <v>1048</v>
       </c>
       <c r="C139" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D139" s="15">
-        <v>130</v>
+        <v>1048</v>
       </c>
       <c r="E139" s="16">
-        <v>44865.584699074076</v>
+        <v>44869.567465277774</v>
       </c>
       <c r="F139" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H139" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B140" s="15">
-        <v>468</v>
+        <v>130</v>
       </c>
       <c r="C140" s="16">
         <v>45533.322013888886</v>
       </c>
       <c r="D140" s="15">
+        <v>130</v>
+      </c>
+      <c r="E140" s="16">
+        <v>44865.584699074076</v>
+      </c>
+      <c r="F140" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H140" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B141" s="15">
         <v>468</v>
       </c>
-      <c r="E140" s="16">
+      <c r="C141" s="16">
+        <v>45533.322013888886</v>
+      </c>
+      <c r="D141" s="15">
+        <v>468</v>
+      </c>
+      <c r="E141" s="16">
         <v>44865.591597222221</v>
       </c>
-      <c r="F140" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H140" s="15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A141" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A142" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B142" s="22">
+      <c r="F141" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H141" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A142" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B143" s="22">
         <v>2387</v>
       </c>
-      <c r="C142" s="23">
+      <c r="C143" s="23">
         <v>45533.322013888886</v>
       </c>
-      <c r="D142" s="22">
+      <c r="D143" s="22">
         <v>2387</v>
       </c>
-      <c r="E142" s="23">
+      <c r="E143" s="23">
         <v>44862.525694444441</v>
       </c>
-      <c r="F142" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A143" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B143" s="13">
+      <c r="F143" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B144" s="13">
         <v>156</v>
       </c>
-      <c r="C143" s="14">
+      <c r="C144" s="14">
         <v>45533.322013888886</v>
       </c>
-      <c r="D143" s="13">
+      <c r="D144" s="13">
         <v>156</v>
       </c>
-      <c r="E143" s="14">
+      <c r="E144" s="14">
         <v>42949.567870370367</v>
       </c>
-      <c r="F143" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A144" s="27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A145" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="F145" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H145" s="13" t="s">
-        <v>236</v>
+      <c r="F144" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A145" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A146" s="13" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F146" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A147" s="29" t="s">
-        <v>232</v>
+      <c r="A147" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="F147" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B148" s="20">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A148" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="F148" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H148" s="13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B149" s="20">
         <v>260</v>
       </c>
-      <c r="C148" s="20">
+      <c r="C149" s="20">
         <v>45533.32203703704</v>
       </c>
-      <c r="D148" s="20">
+      <c r="D149" s="20">
         <v>260</v>
       </c>
-      <c r="E148" s="20">
+      <c r="E149" s="20">
         <v>44865.684282407405</v>
       </c>
-      <c r="F148" s="20" t="s">
+      <c r="F149" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H148" s="20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A149" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C149" s="14"/>
-      <c r="E149" s="14"/>
-      <c r="F149" s="13" t="s">
+      <c r="H149" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="13" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="B150" s="20">
-        <v>265</v>
-      </c>
-      <c r="C150" s="20">
-        <v>45533.32203703704</v>
-      </c>
-      <c r="D150" s="20">
-        <v>265</v>
-      </c>
-      <c r="E150" s="20">
-        <v>44868.638414351852</v>
-      </c>
-      <c r="F150" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H150" s="20" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A151" s="20" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B151" s="20">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C151" s="20">
         <v>45533.32203703704</v>
       </c>
       <c r="D151" s="20">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="E151" s="20">
-        <v>44868.639050925929</v>
+        <v>44868.638414351852</v>
       </c>
       <c r="F151" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H151" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A152" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B152" s="13">
-        <v>1257</v>
-      </c>
-      <c r="C152" s="14">
-        <v>45636.738125000003</v>
-      </c>
-      <c r="D152" s="13">
-        <v>749</v>
-      </c>
-      <c r="E152" s="14">
-        <v>44865.678263888891</v>
-      </c>
-      <c r="F152" s="13" t="s">
-        <v>55</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A152" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B152" s="20">
+        <v>275</v>
+      </c>
+      <c r="C152" s="20">
+        <v>45533.32203703704</v>
+      </c>
+      <c r="D152" s="20">
+        <v>275</v>
+      </c>
+      <c r="E152" s="20">
+        <v>44868.639050925929</v>
+      </c>
+      <c r="F152" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H152" s="20" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A153" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B153" s="13">
+        <v>1257</v>
+      </c>
+      <c r="C153" s="14">
+        <v>45636.738125000003</v>
+      </c>
+      <c r="D153" s="13">
+        <v>749</v>
+      </c>
+      <c r="E153" s="14">
+        <v>44865.678263888891</v>
+      </c>
+      <c r="F153" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A154" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B154" s="13">
+        <v>906</v>
+      </c>
+      <c r="C154" s="14">
+        <v>45636.727048611108</v>
+      </c>
+      <c r="D154" s="13">
+        <v>767</v>
+      </c>
+      <c r="E154" s="14">
+        <v>44865.681134259263</v>
+      </c>
+      <c r="F154" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="B153" s="13">
-        <v>906</v>
-      </c>
-      <c r="C153" s="14">
-        <v>45636.727048611108</v>
-      </c>
-      <c r="D153" s="13">
-        <v>767</v>
-      </c>
-      <c r="E153" s="14">
-        <v>44865.681134259263</v>
-      </c>
-      <c r="F153" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A154" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="B154" s="15">
+      <c r="B155" s="15">
         <v>1057</v>
       </c>
-      <c r="C154" s="16">
+      <c r="C155" s="16">
         <v>45533.322048611109</v>
       </c>
-      <c r="D154" s="15">
+      <c r="D155" s="15">
         <v>1057</v>
       </c>
-      <c r="E154" s="16">
+      <c r="E155" s="16">
         <v>44865.684537037036</v>
       </c>
-      <c r="F154" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H154" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A155" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="B155" s="13">
-        <v>358</v>
-      </c>
-      <c r="C155" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D155" s="13">
-        <v>358</v>
-      </c>
-      <c r="E155" s="14">
-        <v>44865.660231481481</v>
-      </c>
-      <c r="F155" s="13" t="s">
-        <v>11</v>
+      <c r="F155" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H155" s="15" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="156" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" s="13" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B156" s="13">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C156" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D156" s="13">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E156" s="14">
-        <v>44865.659814814811</v>
+        <v>44865.660231481481</v>
       </c>
       <c r="F156" s="13" t="s">
         <v>11</v>
@@ -5809,19 +5637,19 @@
     </row>
     <row r="157" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="13" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B157" s="13">
-        <v>563</v>
+        <v>365</v>
       </c>
       <c r="C157" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D157" s="13">
-        <v>563</v>
+        <v>365</v>
       </c>
       <c r="E157" s="14">
-        <v>44865.672083333331</v>
+        <v>44865.659814814811</v>
       </c>
       <c r="F157" s="13" t="s">
         <v>11</v>
@@ -5829,79 +5657,79 @@
     </row>
     <row r="158" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" s="13" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B158" s="13">
-        <v>253</v>
+        <v>563</v>
       </c>
       <c r="C158" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D158" s="13">
+        <v>563</v>
+      </c>
+      <c r="E158" s="14">
+        <v>44865.672083333331</v>
+      </c>
+      <c r="F158" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A159" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B159" s="13">
         <v>253</v>
       </c>
-      <c r="E158" s="14">
+      <c r="C159" s="14">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D159" s="13">
+        <v>253</v>
+      </c>
+      <c r="E159" s="14">
         <v>44865.664467592593</v>
       </c>
-      <c r="F158" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A159" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B159" s="22">
+      <c r="F159" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A160" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B160" s="22">
         <v>1062</v>
       </c>
-      <c r="C159" s="23">
+      <c r="C160" s="23">
         <v>45533.322048611109</v>
       </c>
-      <c r="D159" s="22">
+      <c r="D160" s="22">
         <v>1062</v>
       </c>
-      <c r="E159" s="23">
+      <c r="E160" s="23">
         <v>44865.663032407407</v>
       </c>
-      <c r="F159" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H159" s="30" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A160" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B160" s="13">
-        <v>499</v>
-      </c>
-      <c r="C160" s="14">
-        <v>45533.322048611109</v>
-      </c>
-      <c r="D160" s="13">
-        <v>499</v>
-      </c>
-      <c r="E160" s="14">
-        <v>44846.595578703702</v>
-      </c>
-      <c r="F160" s="13" t="s">
-        <v>11</v>
+      <c r="F160" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H160" s="30" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B161" s="13">
-        <v>285</v>
+        <v>499</v>
       </c>
       <c r="C161" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D161" s="13">
-        <v>285</v>
+        <v>499</v>
       </c>
       <c r="E161" s="14">
         <v>44846.595578703702</v>
@@ -5912,99 +5740,99 @@
     </row>
     <row r="162" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B162" s="13">
-        <v>989</v>
+        <v>285</v>
       </c>
       <c r="C162" s="14">
         <v>45533.322048611109</v>
       </c>
       <c r="D162" s="13">
+        <v>285</v>
+      </c>
+      <c r="E162" s="14">
+        <v>44846.595578703702</v>
+      </c>
+      <c r="F162" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B163" s="13">
         <v>989</v>
       </c>
-      <c r="E162" s="14">
+      <c r="C163" s="14">
+        <v>45533.322048611109</v>
+      </c>
+      <c r="D163" s="13">
+        <v>989</v>
+      </c>
+      <c r="E163" s="14">
         <v>44865.669976851852</v>
       </c>
-      <c r="F162" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A163" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B163" s="3"/>
-      <c r="C163" s="6"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="6"/>
-      <c r="F163" s="11"/>
-    </row>
-    <row r="164" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A164" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B164" s="13">
+      <c r="F163" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A164" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B164" s="3"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="11"/>
+    </row>
+    <row r="165" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A165" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B165" s="13">
         <v>329</v>
       </c>
-      <c r="C164" s="14">
+      <c r="C165" s="14">
         <v>45637.51290509259</v>
       </c>
-      <c r="D164" s="13">
+      <c r="D165" s="13">
         <v>418</v>
       </c>
-      <c r="E164" s="14">
+      <c r="E165" s="14">
         <v>44869.465717592589</v>
       </c>
-      <c r="F164" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A165" s="28" t="s">
-        <v>138</v>
+      <c r="F165" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="166" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A166" s="28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A167" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B167" s="3">
-        <v>181</v>
-      </c>
-      <c r="C167" s="6">
-        <v>45533.322071759256</v>
-      </c>
-      <c r="D167" s="3">
-        <v>181</v>
-      </c>
-      <c r="E167" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F167" s="11" t="s">
-        <v>11</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A167" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A168" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B168" s="3">
-        <v>242</v>
+        <v>181</v>
       </c>
       <c r="C168" s="6">
         <v>45533.322071759256</v>
       </c>
       <c r="D168" s="3">
-        <v>242</v>
+        <v>181</v>
       </c>
       <c r="E168" s="6">
-        <v>43763.840231481481</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F168" s="11" t="s">
         <v>11</v>
@@ -6012,19 +5840,19 @@
     </row>
     <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A169" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B169" s="3">
-        <v>1778</v>
+        <v>242</v>
       </c>
       <c r="C169" s="6">
         <v>45533.322071759256</v>
       </c>
       <c r="D169" s="3">
-        <v>1778</v>
+        <v>242</v>
       </c>
       <c r="E169" s="6">
-        <v>44868.696817129632</v>
+        <v>43763.840231481481</v>
       </c>
       <c r="F169" s="11" t="s">
         <v>11</v>
@@ -6032,19 +5860,19 @@
     </row>
     <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A170" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B170" s="3">
-        <v>1520</v>
+        <v>1778</v>
       </c>
       <c r="C170" s="6">
-        <v>45533.322083333333</v>
+        <v>45533.322071759256</v>
       </c>
       <c r="D170" s="3">
-        <v>1520</v>
+        <v>1778</v>
       </c>
       <c r="E170" s="6">
-        <v>42949.567847222221</v>
+        <v>44868.696817129632</v>
       </c>
       <c r="F170" s="11" t="s">
         <v>11</v>
@@ -6052,16 +5880,16 @@
     </row>
     <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A171" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B171" s="3">
-        <v>791</v>
+        <v>1520</v>
       </c>
       <c r="C171" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D171" s="3">
-        <v>791</v>
+        <v>1520</v>
       </c>
       <c r="E171" s="6">
         <v>42949.567847222221</v>
@@ -6072,19 +5900,19 @@
     </row>
     <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A172" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B172" s="3">
-        <v>761</v>
+        <v>791</v>
       </c>
       <c r="C172" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D172" s="3">
-        <v>761</v>
+        <v>791</v>
       </c>
       <c r="E172" s="6">
-        <v>42990.771851851852</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F172" s="11" t="s">
         <v>11</v>
@@ -6092,19 +5920,19 @@
     </row>
     <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A173" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B173" s="3">
-        <v>173</v>
+        <v>761</v>
       </c>
       <c r="C173" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D173" s="3">
-        <v>173</v>
+        <v>761</v>
       </c>
       <c r="E173" s="6">
-        <v>42949.567847222221</v>
+        <v>42990.771851851852</v>
       </c>
       <c r="F173" s="11" t="s">
         <v>11</v>
@@ -6112,79 +5940,79 @@
     </row>
     <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A174" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B174" s="3">
-        <v>1710</v>
+        <v>173</v>
       </c>
       <c r="C174" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D174" s="3">
+        <v>173</v>
+      </c>
+      <c r="E174" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F174" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A175" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B175" s="3">
         <v>1710</v>
       </c>
-      <c r="E174" s="6">
+      <c r="C175" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D175" s="3">
+        <v>1710</v>
+      </c>
+      <c r="E175" s="6">
         <v>43711.608078703706</v>
       </c>
-      <c r="F174" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A175" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B175" s="22">
+      <c r="F175" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A176" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B176" s="22">
         <v>3385</v>
       </c>
-      <c r="C175" s="23">
+      <c r="C176" s="23">
         <v>45637.536157407405</v>
       </c>
-      <c r="D175" s="22">
+      <c r="D176" s="22">
         <v>3379</v>
       </c>
-      <c r="E175" s="23">
+      <c r="E176" s="23">
         <v>44865.695879629631</v>
       </c>
-      <c r="F175" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H175" s="22" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A176" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B176" s="3">
-        <v>261</v>
-      </c>
-      <c r="C176" s="6">
-        <v>45533.322083333333</v>
-      </c>
-      <c r="D176" s="3">
-        <v>261</v>
-      </c>
-      <c r="E176" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F176" s="11" t="s">
-        <v>11</v>
+      <c r="F176" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H176" s="22" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A177" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B177" s="3">
-        <v>876</v>
+        <v>261</v>
       </c>
       <c r="C177" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D177" s="3">
-        <v>876</v>
+        <v>261</v>
       </c>
       <c r="E177" s="6">
         <v>42949.567847222221</v>
@@ -6195,19 +6023,19 @@
     </row>
     <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A178" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B178" s="3">
-        <v>571</v>
+        <v>876</v>
       </c>
       <c r="C178" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D178" s="3">
-        <v>571</v>
+        <v>876</v>
       </c>
       <c r="E178" s="6">
-        <v>44076.622754629629</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F178" s="11" t="s">
         <v>11</v>
@@ -6215,82 +6043,82 @@
     </row>
     <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A179" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B179" s="3">
-        <v>1122</v>
+        <v>571</v>
       </c>
       <c r="C179" s="6">
         <v>45533.322083333333</v>
       </c>
       <c r="D179" s="3">
+        <v>571</v>
+      </c>
+      <c r="E179" s="6">
+        <v>44076.622754629629</v>
+      </c>
+      <c r="F179" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A180" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B180" s="3">
         <v>1122</v>
       </c>
-      <c r="E179" s="6">
+      <c r="C180" s="6">
+        <v>45533.322083333333</v>
+      </c>
+      <c r="D180" s="3">
+        <v>1122</v>
+      </c>
+      <c r="E180" s="6">
         <v>44861.716111111113</v>
       </c>
-      <c r="F179" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A180" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B180" s="15">
+      <c r="F180" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A181" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B181" s="15">
         <v>1885</v>
       </c>
-      <c r="C180" s="16">
+      <c r="C181" s="16">
         <v>45533.322094907409</v>
       </c>
-      <c r="D180" s="15">
+      <c r="D181" s="15">
         <v>1932</v>
       </c>
-      <c r="E180" s="16">
+      <c r="E181" s="16">
         <v>44852.752916666665</v>
       </c>
-      <c r="F180" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H180" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A181" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B181" s="3">
-        <v>1328</v>
-      </c>
-      <c r="C181" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D181" s="3">
-        <v>1328</v>
-      </c>
-      <c r="E181" s="6">
-        <v>42949.567847222221</v>
-      </c>
-      <c r="F181" s="11" t="s">
-        <v>11</v>
+      <c r="F181" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H181" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A182" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B182" s="3">
-        <v>318</v>
+        <v>1328</v>
       </c>
       <c r="C182" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D182" s="3">
-        <v>318</v>
+        <v>1328</v>
       </c>
       <c r="E182" s="6">
-        <v>42990.77134259259</v>
+        <v>42949.567847222221</v>
       </c>
       <c r="F182" s="11" t="s">
         <v>11</v>
@@ -6298,19 +6126,19 @@
     </row>
     <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A183" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B183" s="3">
-        <v>1009</v>
+        <v>318</v>
       </c>
       <c r="C183" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D183" s="3">
-        <v>1009</v>
+        <v>318</v>
       </c>
       <c r="E183" s="6">
-        <v>44852.670138888891</v>
+        <v>42990.77134259259</v>
       </c>
       <c r="F183" s="11" t="s">
         <v>11</v>
@@ -6318,19 +6146,19 @@
     </row>
     <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A184" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B184" s="3">
-        <v>1657</v>
+        <v>1009</v>
       </c>
       <c r="C184" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D184" s="3">
-        <v>1657</v>
+        <v>1009</v>
       </c>
       <c r="E184" s="6">
-        <v>42990.765023148146</v>
+        <v>44852.670138888891</v>
       </c>
       <c r="F184" s="11" t="s">
         <v>11</v>
@@ -6338,79 +6166,79 @@
     </row>
     <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A185" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B185" s="3">
+        <v>1657</v>
+      </c>
+      <c r="C185" s="6">
+        <v>45533.322094907409</v>
+      </c>
+      <c r="D185" s="3">
+        <v>1657</v>
+      </c>
+      <c r="E185" s="6">
+        <v>42990.765023148146</v>
+      </c>
+      <c r="F185" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A186" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B185" s="3">
+      <c r="B186" s="3">
         <v>1677</v>
       </c>
-      <c r="C185" s="6">
+      <c r="C186" s="6">
         <v>45533.322083333333</v>
       </c>
-      <c r="D185" s="3">
+      <c r="D186" s="3">
         <v>1677</v>
       </c>
-      <c r="E185" s="6">
+      <c r="E186" s="6">
         <v>44848.55972222222</v>
       </c>
-      <c r="F185" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A186" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B186" s="13">
+      <c r="F186" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A187" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B187" s="13">
         <v>2576</v>
       </c>
-      <c r="C186" s="14">
+      <c r="C187" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D186" s="13">
+      <c r="D187" s="13">
         <v>2576</v>
       </c>
-      <c r="E186" s="14">
+      <c r="E187" s="14">
         <v>43304.752638888887</v>
       </c>
-      <c r="F186" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A187" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B187" s="3">
-        <v>1237</v>
-      </c>
-      <c r="C187" s="6">
-        <v>45533.322094907409</v>
-      </c>
-      <c r="D187" s="3">
-        <v>1237</v>
-      </c>
-      <c r="E187" s="6">
-        <v>43710.58252314815</v>
-      </c>
-      <c r="F187" s="11" t="s">
-        <v>11</v>
+      <c r="F187" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A188" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B188" s="3">
-        <v>872</v>
+        <v>1237</v>
       </c>
       <c r="C188" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D188" s="3">
-        <v>872</v>
+        <v>1237</v>
       </c>
       <c r="E188" s="6">
-        <v>42949.567847222221</v>
+        <v>43710.58252314815</v>
       </c>
       <c r="F188" s="11" t="s">
         <v>11</v>
@@ -6418,352 +6246,358 @@
     </row>
     <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A189" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B189" s="3">
-        <v>2471</v>
+        <v>872</v>
       </c>
       <c r="C189" s="6">
         <v>45533.322094907409</v>
       </c>
       <c r="D189" s="3">
+        <v>872</v>
+      </c>
+      <c r="E189" s="6">
+        <v>42949.567847222221</v>
+      </c>
+      <c r="F189" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A190" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B190" s="3">
         <v>2471</v>
       </c>
-      <c r="E189" s="6">
+      <c r="C190" s="6">
+        <v>45533.322094907409</v>
+      </c>
+      <c r="D190" s="3">
+        <v>2471</v>
+      </c>
+      <c r="E190" s="6">
         <v>42949.567870370367</v>
       </c>
-      <c r="F189" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A190" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="B190" s="3"/>
-      <c r="C190" s="6"/>
-      <c r="D190" s="3"/>
-      <c r="E190" s="6"/>
-      <c r="F190" s="11"/>
-    </row>
-    <row r="191" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A191" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B191" s="13">
+      <c r="F190" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A191" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B191" s="3"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="11"/>
+    </row>
+    <row r="192" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A192" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B192" s="13">
         <v>492</v>
       </c>
-      <c r="C191" s="14">
+      <c r="C192" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D191" s="13">
+      <c r="D192" s="13">
         <v>492</v>
       </c>
-      <c r="E191" s="14">
+      <c r="E192" s="14">
         <v>44868.679872685185</v>
       </c>
-      <c r="F191" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A192" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B192" s="3">
+      <c r="F192" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A193" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B193" s="15">
         <v>1135</v>
       </c>
-      <c r="C192" s="6">
+      <c r="C193" s="16">
         <v>45637.672824074078</v>
       </c>
-      <c r="D192" s="3">
+      <c r="D193" s="15">
         <v>1267</v>
       </c>
-      <c r="E192" s="6">
+      <c r="E193" s="16">
         <v>44869.576215277775</v>
       </c>
-      <c r="F192" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A193" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B193" s="3">
+      <c r="F193" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H193" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A194" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B194" s="13">
         <v>3316</v>
       </c>
-      <c r="C193" s="6">
+      <c r="C194" s="14">
         <v>45533.322094907409</v>
       </c>
-      <c r="D193" s="3">
+      <c r="D194" s="13">
         <v>3316</v>
       </c>
-      <c r="E193" s="6">
+      <c r="E194" s="14">
         <v>44869.449074074073</v>
       </c>
-      <c r="F193" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A194" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B194" s="3">
-        <v>2293</v>
-      </c>
-      <c r="C194" s="6">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D194" s="3">
-        <v>2293</v>
-      </c>
-      <c r="E194" s="6">
-        <v>44869.446643518517</v>
-      </c>
-      <c r="F194" s="11" t="s">
+      <c r="F194" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A195" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B195" s="3">
-        <v>2288</v>
+        <v>2293</v>
       </c>
       <c r="C195" s="6">
         <v>45533.322106481479</v>
       </c>
       <c r="D195" s="3">
+        <v>2293</v>
+      </c>
+      <c r="E195" s="6">
+        <v>44869.446643518517</v>
+      </c>
+      <c r="F195" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A196" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B196" s="13">
         <v>2288</v>
       </c>
-      <c r="E195" s="6">
+      <c r="C196" s="14">
+        <v>45533.322106481479</v>
+      </c>
+      <c r="D196" s="13">
+        <v>2288</v>
+      </c>
+      <c r="E196" s="14">
         <v>42949.567847222221</v>
       </c>
-      <c r="F195" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A196" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B196" s="3">
+      <c r="F196" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B197" s="13">
         <v>364</v>
       </c>
-      <c r="C196" s="6">
+      <c r="C197" s="14">
         <v>45533.322106481479</v>
       </c>
-      <c r="D196" s="3">
+      <c r="D197" s="13">
         <v>364</v>
       </c>
-      <c r="E196" s="6">
+      <c r="E197" s="14">
         <v>43863.785486111112</v>
       </c>
-      <c r="F196" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A197" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B197" s="3"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="6"/>
-      <c r="F197" s="11"/>
-    </row>
-    <row r="198" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B198" s="22">
+      <c r="F197" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A198" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B198" s="3"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="3"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="11"/>
+    </row>
+    <row r="199" spans="1:8" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A199" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B199" s="15">
         <v>4763</v>
       </c>
-      <c r="C198" s="23">
+      <c r="C199" s="16">
         <v>45622.614722222221</v>
       </c>
-      <c r="D198" s="22">
+      <c r="D199" s="15">
         <v>4832</v>
       </c>
-      <c r="E198" s="23">
+      <c r="E199" s="16">
         <v>44869.413148148145</v>
       </c>
-      <c r="F198" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H198" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="B199" s="13">
-        <v>483</v>
-      </c>
-      <c r="C199" s="14">
-        <v>45533.322106481479</v>
-      </c>
-      <c r="D199" s="13">
-        <v>483</v>
-      </c>
-      <c r="E199" s="14">
-        <v>42992.768796296295</v>
-      </c>
-      <c r="F199" s="13" t="s">
-        <v>11</v>
+      <c r="F199" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H199" s="15" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="200" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A200" s="13" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B200" s="13">
-        <v>743</v>
+        <v>483</v>
       </c>
       <c r="C200" s="14">
-        <v>45637.479016203702</v>
+        <v>45533.322106481479</v>
       </c>
       <c r="D200" s="13">
-        <v>836</v>
+        <v>483</v>
       </c>
       <c r="E200" s="14">
-        <v>44869.403402777774</v>
+        <v>42992.768796296295</v>
       </c>
       <c r="F200" s="13" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A201" s="13" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B201" s="13">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="C201" s="14">
-        <v>45637.479409722226</v>
+        <v>45637.479016203702</v>
       </c>
       <c r="D201" s="13">
-        <v>761</v>
+        <v>836</v>
       </c>
       <c r="E201" s="14">
-        <v>44869.396956018521</v>
+        <v>44869.403402777774</v>
       </c>
       <c r="F201" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="202" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A202" s="13" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="B202" s="13">
+        <v>749</v>
+      </c>
+      <c r="C202" s="14">
+        <v>45637.479409722226</v>
+      </c>
+      <c r="D202" s="13">
+        <v>761</v>
+      </c>
+      <c r="E202" s="14">
+        <v>44869.396956018521</v>
+      </c>
+      <c r="F202" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A203" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B203" s="13">
         <v>451</v>
       </c>
-      <c r="C202" s="14">
+      <c r="C203" s="14">
         <v>45637.539085648146</v>
       </c>
-      <c r="D202" s="13">
+      <c r="D203" s="13">
         <v>401</v>
       </c>
-      <c r="E202" s="14">
+      <c r="E203" s="14">
         <v>42999.700740740744</v>
       </c>
-      <c r="F202" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A203" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B203" s="3"/>
-      <c r="C203" s="6"/>
-      <c r="D203" s="3"/>
-      <c r="E203" s="6"/>
-      <c r="F203" s="11"/>
-    </row>
-    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A204" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B204" s="3">
+      <c r="F203" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A204" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B204" s="3"/>
+      <c r="C204" s="6"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="6"/>
+      <c r="F204" s="11"/>
+    </row>
+    <row r="205" spans="1:8" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A205" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B205" s="22">
         <v>815</v>
       </c>
-      <c r="C204" s="6">
+      <c r="C205" s="23">
         <v>45533.322106481479</v>
       </c>
-      <c r="D204" s="3">
+      <c r="D205" s="22">
         <v>815</v>
       </c>
-      <c r="E204" s="6">
+      <c r="E205" s="23">
         <v>44865.586435185185</v>
       </c>
-      <c r="F204" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A205" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B205" s="3">
-        <v>2674</v>
-      </c>
-      <c r="C205" s="6">
-        <v>45637.463252314818</v>
-      </c>
-      <c r="D205" s="3">
-        <v>2649</v>
-      </c>
-      <c r="E205" s="6">
-        <v>44869.507557870369</v>
-      </c>
-      <c r="F205" s="11" t="s">
-        <v>56</v>
+      <c r="F205" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H205" s="22" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A206" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B206" s="3">
-        <v>162</v>
+        <v>2674</v>
       </c>
       <c r="C206" s="6">
-        <v>45533.322118055556</v>
+        <v>45637.463252314818</v>
       </c>
       <c r="D206" s="3">
-        <v>162</v>
+        <v>2649</v>
       </c>
       <c r="E206" s="6">
-        <v>42949.567870370367</v>
+        <v>44869.507557870369</v>
       </c>
       <c r="F206" s="11" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A207" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B207" s="3">
-        <v>286</v>
+        <v>162</v>
       </c>
       <c r="C207" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D207" s="3">
-        <v>286</v>
+        <v>162</v>
       </c>
       <c r="E207" s="6">
-        <v>44861.727037037039</v>
+        <v>42949.567870370367</v>
       </c>
       <c r="F207" s="11" t="s">
         <v>11</v>
@@ -6771,19 +6605,19 @@
     </row>
     <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A208" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B208" s="3">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="C208" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D208" s="3">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="E208" s="6">
-        <v>44861.727152777778</v>
+        <v>44861.727037037039</v>
       </c>
       <c r="F208" s="11" t="s">
         <v>11</v>
@@ -6791,19 +6625,19 @@
     </row>
     <row r="209" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A209" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B209" s="3">
-        <v>420</v>
+        <v>255</v>
       </c>
       <c r="C209" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D209" s="3">
-        <v>420</v>
+        <v>255</v>
       </c>
       <c r="E209" s="6">
-        <v>44861.727546296293</v>
+        <v>44861.727152777778</v>
       </c>
       <c r="F209" s="11" t="s">
         <v>11</v>
@@ -6811,60 +6645,66 @@
     </row>
     <row r="210" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A210" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B210" s="3">
-        <v>138</v>
+        <v>420</v>
       </c>
       <c r="C210" s="6">
         <v>45533.322118055556</v>
       </c>
       <c r="D210" s="3">
+        <v>420</v>
+      </c>
+      <c r="E210" s="6">
+        <v>44861.727546296293</v>
+      </c>
+      <c r="F210" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A211" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B211" s="3">
         <v>138</v>
       </c>
-      <c r="E210" s="6">
+      <c r="C211" s="6">
+        <v>45533.322118055556</v>
+      </c>
+      <c r="D211" s="3">
+        <v>138</v>
+      </c>
+      <c r="E211" s="6">
         <v>44869.508900462963</v>
       </c>
-      <c r="F210" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A211" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B211" s="22">
+      <c r="F211" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" s="22" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A212" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B212" s="22">
         <v>11219</v>
       </c>
-      <c r="C211" s="23">
+      <c r="C212" s="23">
         <v>45636.606886574074</v>
       </c>
-      <c r="D211" s="22">
+      <c r="D212" s="22">
         <v>13055</v>
       </c>
-      <c r="E211" s="23">
+      <c r="E212" s="23">
         <v>44869.593541666669</v>
       </c>
-      <c r="F211" s="22" t="s">
-        <v>55</v>
+      <c r="F212" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B7:C7"/>
@@ -6877,18 +6717,40 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B81:C81"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D104 A105:B106 D105:E106 A107:E107 A108:B112 D108:E112 A113:E119 A120:D120 B121:D123 A124:D124 A125:E146 B147:E147 A148:E211">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="/.">
+  <conditionalFormatting sqref="A6:G6 B7 D7 F7 A8:F9 A10:B25 D10:E25 A26:F34 B35:F35 A36:F66 A67:B68 D67:E68 A69:F74 A75:B75 D75:E75 A76:F76 A77:B77 D77:E77 A78:D78 A79:E79 A80:D80 A81:B81 D81:E81 A82:E93 A94:B94 D94:E94 A95:E102 A103:D104 A106:B107 D106:E107 A108:E108 A109:B113 D109:E113 A114:E120 A121:D121 B122:D124 A125:D125 A126:E147 B148:E148 A149:E212">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="/.">
       <formula>NOT(ISERROR(SEARCH("/.",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 B121:E123 A124:E146 B147:E147 A148:E211 G159 I159:XFD159 G160:XFD211 A212:XFD1048576 A77:E120 G77:XFD158">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="removed">
+  <conditionalFormatting sqref="A1:XFD9 A10:E25 G10:XFD25 A26:XFD26 A27:G34 I27:XFD56 B35:G35 A36:G56 A57:XFD63 A64:G64 I64:XFD64 A65:XFD66 A67:E68 G67:XFD68 A69:XFD74 A75:E75 G75:XFD75 A76:XFD76 A77:E104 G77:XFD104 A106:E121 G106:XFD159 B122:E124 A125:E147 B148:E148 A149:E212 G160 I160:XFD160 G161:XFD212 A213:XFD1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="added">
+      <formula>NOT(ISERROR(SEARCH("added",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H105">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="removed">
+      <formula>NOT(ISERROR(SEARCH("removed",H105)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="added">
-      <formula>NOT(ISERROR(SEARCH("added",A1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("added",H105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6901,17 +6763,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="J1" s="32" t="s">
         <v>240</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>